<commit_message>
Optimized stat significance by using skellam model
</commit_message>
<xml_diff>
--- a/SRS.dashboard.template.xlsx
+++ b/SRS.dashboard.template.xlsx
@@ -14,15 +14,15 @@
     <sheet name="Lookups" r:id="rId5" sheetId="5"/>
   </sheets>
   <definedNames>
-    <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$2100</definedName>
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$CB$1</definedName>
-    <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="cuts_head">'Lookups'!$F$1:$O$1</definedName>
-    <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$2100</definedName>
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
-    <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
-    <definedName name="zero_string">'Lookups'!$P$1</definedName>
+    <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$CB$1</definedName>
+    <definedName name="disp_value_values">'DisplayValues'!$B$2:$CB$151</definedName>
+    <definedName name="cuts_config">'Lookups'!$A$1:$D$1</definedName>
+    <definedName name="default_mapping">'Lookups'!$D$2:$E$101</definedName>
+    <definedName name="cuts_head">'Lookups'!$E$1:$L$1</definedName>
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$CB$1</definedName>
     <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$151</definedName>
     <definedName name="disp_value_values">'DisplayValues'!$B$2:$CB$151</definedName>
@@ -1571,28 +1571,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF800000"/>
-      <name val="DINOT-Bold"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF800000"/>
       <name val="DINOT-Regular"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF800000"/>
-      <name val="DINOT-Regular"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF993366"/>
-      <name val="DINOT-Regular"/>
-      <family val="2"/>
+      <b/>
     </font>
     <font>
       <sz val="12"/>
@@ -1607,32 +1590,31 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF800000"/>
-      <name val="DINOT-Regular"/>
-      <family val="2"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <color rgb="FF800000"/>
       <name val="DINOT-Bold"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF800000"/>
       <name val="DINOT-Regular"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF800000"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF993366"/>
+      <name val="DINOT-Regular"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="DINOT-Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF800000"/>
       <name val="DINOT-Regular"/>
       <family val="2"/>
@@ -1646,15 +1628,33 @@
       <b/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF00FF"/>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF800000"/>
+      <name val="DINOT-Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
       <name val="DINOT-Regular"/>
       <family val="2"/>
       <b/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <color rgb="FF800000"/>
+      <name val="DINOT-Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF00FF"/>
       <name val="DINOT-Regular"/>
       <family val="2"/>
       <b/>
@@ -1669,6 +1669,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="6" tint="-0.24994659260841701"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3737"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FF00CCFF"/>
       </patternFill>
@@ -1680,18 +1697,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="mediumGray">
-        <fgColor rgb="FF3366FF"/>
-        <bgColor rgb="FF008000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCFF"/>
         <bgColor rgb="FF3366FF"/>
@@ -1699,13 +1704,8 @@
     </fill>
     <fill>
       <patternFill patternType="mediumGray">
-        <bgColor theme="6" tint="-0.24994659260841701"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3737"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF3366FF"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1723,95 +1723,15 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFFFFFCC"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color rgb="FFFFFFCC"/>
+        <color rgb="FF800000"/>
       </right>
       <top style="thin">
         <color rgb="FF800000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000080"/>
-      </right>
-      <top/>
       <bottom style="thin">
-        <color rgb="FFFFFFCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF800000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF800000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000080"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1844,15 +1764,93 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000080"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFCC"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF800000"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF800000"/>
+      </right>
+      <top style="thin">
         <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF800000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFCC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000080"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1864,6 +1862,73 @@
         <color rgb="FF800000"/>
       </right>
       <top style="thin">
+        <color rgb="FF800000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF800000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFCC"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF800000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF800000"/>
+      </right>
+      <top style="medium">
         <color rgb="FF800000"/>
       </top>
       <bottom/>
@@ -1902,19 +1967,6 @@
       <right style="thin">
         <color rgb="FFFFFFCC"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFFFFCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFCC"/>
-      </right>
       <top style="thin">
         <color rgb="FFFFFFCC"/>
       </top>
@@ -1924,16 +1976,77 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFCC"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF800000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFFFFFCC"/>
       </left>
       <right/>
       <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF800000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF800000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000080"/>
+      </right>
+      <top style="thin">
         <color rgb="FFFFFFCC"/>
       </top>
-      <bottom style="hair">
-        <color rgb="FF000080"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1952,50 +2065,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF800000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF800000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF800000"/>
       </left>
@@ -2009,28 +2078,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color rgb="FFFFFFCC"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="hair">
+        <color rgb="FF000080"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF800000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFFFFFCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FFFFFFCC"/>
       </bottom>
@@ -2046,16 +2100,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FFFFFFCC"/>
+      </left>
       <right style="thin">
-        <color rgb="FF800000"/>
+        <color rgb="FFFFFFCC"/>
       </right>
       <top style="thin">
         <color rgb="FF800000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF800000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2072,47 +2126,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFFFFFCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFCC"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF800000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF800000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF800000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFCC"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF800000"/>
       </top>
@@ -2136,39 +2155,13 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF800000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FFFFFFCC"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFCC"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000080"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFFFFCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFCC"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF800000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2185,17 +2178,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF800000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF800000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2205,179 +2205,179 @@
   </cellStyleXfs>
   <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="5" fillId="5" fontId="4" numFmtId="49" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="0" fontId="4" numFmtId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="8" fillId="5" fontId="6" numFmtId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="5" fontId="7" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="2" fontId="4" numFmtId="1" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="10" fillId="5" fontId="6" numFmtId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="5" fillId="0" fontId="5" numFmtId="9" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="12" fillId="0" fontId="2" numFmtId="165" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="3" fontId="6" numFmtId="1" xfId="0">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="13" fillId="2" fontId="8" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="14" fillId="5" fontId="6" numFmtId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="5" fillId="5" fontId="9" numFmtId="9" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="15" fillId="5" fontId="6" numFmtId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="7" numFmtId="166" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="16" fillId="2" fontId="8" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="17" fillId="5" fontId="4" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="7" fillId="2" fontId="4" numFmtId="1" xfId="0">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="7" numFmtId="1" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="18" fillId="2" fontId="8" numFmtId="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="19" fillId="5" fontId="4" numFmtId="167" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="20" fillId="0" fontId="7" numFmtId="49" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="21" fillId="6" fontId="3" numFmtId="1" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="22" fillId="0" fontId="4" numFmtId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="7" numFmtId="49" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="23" fillId="0" fontId="10" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="7" fontId="11" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="24" fillId="6" fontId="3" numFmtId="1" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="25" fillId="0" fontId="2" numFmtId="9" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="26" fillId="0" fontId="7" numFmtId="49" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="8" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="27" fillId="6" fontId="3" numFmtId="1" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="28" fillId="0" fontId="7" numFmtId="49" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="29" fillId="2" fontId="13" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="30" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="31" fillId="9" fontId="2" numFmtId="9" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="28" fillId="0" fontId="5" numFmtId="49" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="32" fillId="6" fontId="3" numFmtId="1" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="33" fillId="5" fontId="6" numFmtId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="34" fillId="0" fontId="4" numFmtId="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="35" fillId="2" fontId="8" numFmtId="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="17" fillId="0" fontId="14" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="168" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="4" fontId="6" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="3" numFmtId="1" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="10" fillId="3" fontId="6" numFmtId="1" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="36" fillId="6" fontId="3" numFmtId="1" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="12" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="37" fillId="2" fontId="8" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="13" fillId="5" fontId="7" numFmtId="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="31" fillId="0" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="14" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="6" fontId="8" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="15" fillId="2" fontId="1" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="16" fillId="2" fontId="4" numFmtId="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="17" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="3" numFmtId="165" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="18" fillId="5" fontId="7" numFmtId="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="19" fillId="0" fontId="10" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="7" fontId="6" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="20" fillId="0" fontId="1" numFmtId="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="21" fillId="2" fontId="4" numFmtId="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="22" fillId="3" fontId="6" numFmtId="1" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="23" fillId="5" fontId="7" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="24" fillId="2" fontId="1" numFmtId="166" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="8" fontId="6" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="25" fillId="5" fontId="9" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="26" fillId="8" fontId="6" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="27" fillId="0" fontId="5" numFmtId="9" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="26" fillId="7" fontId="6" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="28" fillId="0" fontId="5" numFmtId="167" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="27" fillId="9" fontId="5" numFmtId="9" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="168" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="29" fillId="5" fontId="7" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="15" fillId="2" fontId="12" numFmtId="9" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="30" fillId="0" fontId="1" numFmtId="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="31" fillId="3" fontId="6" numFmtId="1" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="32" fillId="2" fontId="4" numFmtId="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="33" fillId="0" fontId="1" numFmtId="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="12" fillId="0" fontId="13" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="34" fillId="0" fontId="3" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="34" fillId="0" fontId="2" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="35" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="36" fillId="5" fontId="7" numFmtId="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="37" fillId="3" fontId="6" numFmtId="1" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2686,447 +2686,447 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" customWidth="true" max="5" width="9.1640625"/>
-    <col min="4" customWidth="true" max="4" width="9.1640625"/>
-    <col min="7" customWidth="true" max="7" width="9.1640625"/>
-    <col min="6" customWidth="true" max="6" width="9.1640625"/>
-    <col min="1" customWidth="true" max="1" width="9.1640625"/>
-    <col min="3" customWidth="true" max="3" width="16.0"/>
-    <col min="2" customWidth="true" max="2" width="11.5"/>
-    <col min="13" customWidth="true" max="13" width="9.1640625"/>
-    <col min="12" customWidth="true" max="12" width="10.5"/>
-    <col min="15" customWidth="true" max="15" width="9.1640625"/>
-    <col min="14" customWidth="true" max="14" width="9.1640625"/>
-    <col min="9" customWidth="true" max="9" width="9.1640625"/>
-    <col min="8" customWidth="true" max="8" width="10.5"/>
-    <col min="11" customWidth="true" max="11" width="9.1640625"/>
-    <col min="10" customWidth="true" max="10" width="9.1640625"/>
+    <col min="5" width="9.1640625" max="5" customWidth="true"/>
+    <col min="4" width="9.1640625" max="4" customWidth="true"/>
+    <col min="7" width="9.1640625" max="7" customWidth="true"/>
+    <col min="6" width="9.1640625" max="6" customWidth="true"/>
+    <col min="1" width="9.1640625" max="1" customWidth="true"/>
+    <col min="3" width="16.0" max="3" customWidth="true"/>
+    <col min="2" width="11.5" max="2" customWidth="true"/>
+    <col min="13" width="9.1640625" max="13" customWidth="true"/>
+    <col min="12" width="10.5" max="12" customWidth="true"/>
+    <col min="15" width="9.1640625" max="15" customWidth="true"/>
+    <col min="14" width="9.1640625" max="14" customWidth="true"/>
+    <col min="9" width="9.1640625" max="9" customWidth="true"/>
+    <col min="8" width="10.5" max="8" customWidth="true"/>
+    <col min="11" width="9.1640625" max="11" customWidth="true"/>
+    <col min="10" width="9.1640625" max="10" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="C1" s="15" t="s"/>
-      <c r="D1" s="11" t="s"/>
-      <c r="E1" s="11" t="s"/>
-      <c r="F1" s="11" t="s"/>
-      <c r="G1" s="26" t="s"/>
-      <c r="H1" s="15" t="s">
+      <c r="C1" s="49" t="s"/>
+      <c r="D1" s="25" t="s"/>
+      <c r="E1" s="25" t="s"/>
+      <c r="F1" s="25" t="s"/>
+      <c r="G1" s="22" t="s"/>
+      <c r="H1" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="49" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="C2" s="15" t="s"/>
-      <c r="D2" s="15" t="s"/>
-      <c r="E2" s="15" t="s"/>
-      <c r="F2" s="15" t="s"/>
-      <c r="G2" s="15" t="s"/>
-      <c r="H2" s="15" t="s">
+      <c r="C2" s="49" t="s"/>
+      <c r="D2" s="49" t="s"/>
+      <c r="E2" s="49" t="s"/>
+      <c r="F2" s="49" t="s"/>
+      <c r="G2" s="49" t="s"/>
+      <c r="H2" s="49" t="s">
         <v>243</v>
       </c>
-      <c r="I2" s="15" t="e">
+      <c r="I2" s="49" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J2" s="15" t="e">
+      <c r="J2" s="49" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K2" s="15" t="e">
+      <c r="K2" s="49" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="49" t="s">
         <v>243</v>
       </c>
-      <c r="M2" s="15" t="e">
+      <c r="M2" s="49" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N2" s="15" t="e">
+      <c r="N2" s="49" t="e">
         <v>#N/A</v>
       </c>
-      <c r="O2" s="15" t="e">
+      <c r="O2" s="49" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C3" s="15" t="s"/>
-      <c r="D3" s="8" t="s"/>
-      <c r="E3" s="8" t="s"/>
-      <c r="F3" s="8" t="s"/>
-      <c r="G3" s="44" t="s"/>
-      <c r="H3" s="8" t="s">
+      <c r="C3" s="49" t="s"/>
+      <c r="D3" s="5" t="s"/>
+      <c r="E3" s="5" t="s"/>
+      <c r="F3" s="5" t="s"/>
+      <c r="G3" s="55" t="s"/>
+      <c r="H3" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="5" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="C4" s="15" t="s"/>
-      <c r="D4" s="15" t="s"/>
-      <c r="E4" s="15" t="s"/>
-      <c r="F4" s="15" t="s"/>
-      <c r="G4" s="26" t="s"/>
-      <c r="H4" s="15" t="s"/>
-      <c r="I4" s="15" t="s"/>
-      <c r="J4" s="15" t="s"/>
-      <c r="K4" s="15" t="s"/>
-      <c r="L4" s="15" t="s"/>
-      <c r="M4" s="15" t="s"/>
-      <c r="N4" s="15" t="s"/>
-      <c r="O4" s="15" t="s"/>
+      <c r="C4" s="49" t="s"/>
+      <c r="D4" s="49" t="s"/>
+      <c r="E4" s="49" t="s"/>
+      <c r="F4" s="49" t="s"/>
+      <c r="G4" s="22" t="s"/>
+      <c r="H4" s="49" t="s"/>
+      <c r="I4" s="49" t="s"/>
+      <c r="J4" s="49" t="s"/>
+      <c r="K4" s="49" t="s"/>
+      <c r="L4" s="49" t="s"/>
+      <c r="M4" s="49" t="s"/>
+      <c r="N4" s="49" t="s"/>
+      <c r="O4" s="49" t="s"/>
     </row>
     <row r="5" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C5" s="15" t="s"/>
-      <c r="D5" s="15" t="s"/>
-      <c r="E5" s="15" t="s"/>
-      <c r="F5" s="15" t="s"/>
-      <c r="G5" s="26" t="s"/>
-      <c r="H5" s="56" t="s"/>
-      <c r="I5" s="19" t="s"/>
-      <c r="J5" s="19" t="s"/>
-      <c r="K5" s="19" t="s"/>
-      <c r="L5" s="56" t="s"/>
-      <c r="M5" s="19" t="s"/>
-      <c r="N5" s="19" t="s"/>
-      <c r="O5" s="19" t="s"/>
+      <c r="C5" s="49" t="s"/>
+      <c r="D5" s="49" t="s"/>
+      <c r="E5" s="49" t="s"/>
+      <c r="F5" s="49" t="s"/>
+      <c r="G5" s="22" t="s"/>
+      <c r="H5" s="40" t="s"/>
+      <c r="I5" s="2" t="s"/>
+      <c r="J5" s="2" t="s"/>
+      <c r="K5" s="2" t="s"/>
+      <c r="L5" s="40" t="s"/>
+      <c r="M5" s="2" t="s"/>
+      <c r="N5" s="2" t="s"/>
+      <c r="O5" s="2" t="s"/>
     </row>
     <row r="6" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="D6" s="19" t="s"/>
-      <c r="E6" s="15" t="s"/>
-      <c r="F6" s="15" t="s"/>
-      <c r="G6" s="26" t="s"/>
-      <c r="H6" s="56" t="s"/>
-      <c r="I6" s="19" t="s"/>
-      <c r="J6" s="19" t="s"/>
-      <c r="K6" s="19" t="s"/>
-      <c r="L6" s="56" t="s"/>
-      <c r="M6" s="19" t="s"/>
-      <c r="N6" s="19" t="s"/>
-      <c r="O6" s="19" t="s"/>
+      <c r="D6" s="2" t="s"/>
+      <c r="E6" s="49" t="s"/>
+      <c r="F6" s="49" t="s"/>
+      <c r="G6" s="22" t="s"/>
+      <c r="H6" s="40" t="s"/>
+      <c r="I6" s="2" t="s"/>
+      <c r="J6" s="2" t="s"/>
+      <c r="K6" s="2" t="s"/>
+      <c r="L6" s="40" t="s"/>
+      <c r="M6" s="2" t="s"/>
+      <c r="N6" s="2" t="s"/>
+      <c r="O6" s="2" t="s"/>
     </row>
     <row r="7" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="39" t="s">
         <v>432</v>
       </c>
-      <c r="D7" s="19" t="s"/>
-      <c r="E7" s="15" t="s"/>
-      <c r="F7" s="15" t="s"/>
-      <c r="G7" s="26" t="s"/>
-      <c r="H7" s="56" t="s"/>
-      <c r="I7" s="19" t="s"/>
-      <c r="J7" s="19" t="s"/>
-      <c r="K7" s="19" t="s"/>
-      <c r="L7" s="56" t="s"/>
-      <c r="M7" s="19" t="s"/>
-      <c r="N7" s="19" t="s"/>
-      <c r="O7" s="19" t="s"/>
+      <c r="D7" s="2" t="s"/>
+      <c r="E7" s="49" t="s"/>
+      <c r="F7" s="49" t="s"/>
+      <c r="G7" s="22" t="s"/>
+      <c r="H7" s="40" t="s"/>
+      <c r="I7" s="2" t="s"/>
+      <c r="J7" s="2" t="s"/>
+      <c r="K7" s="2" t="s"/>
+      <c r="L7" s="40" t="s"/>
+      <c r="M7" s="2" t="s"/>
+      <c r="N7" s="2" t="s"/>
+      <c r="O7" s="2" t="s"/>
     </row>
     <row r="8" customHeight="1" ht="32.25" spans="1:15">
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="18" t="s">
         <v>495</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="26" t="s">
         <v>492</v>
       </c>
-      <c r="E8" s="28" t="s"/>
-      <c r="F8" s="28" t="s"/>
-      <c r="G8" s="57" t="s"/>
-      <c r="H8" s="40" t="s">
+      <c r="E8" s="57" t="s"/>
+      <c r="F8" s="57" t="s"/>
+      <c r="G8" s="51" t="s"/>
+      <c r="H8" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="I8" s="30" t="s"/>
-      <c r="J8" s="30" t="s"/>
-      <c r="K8" s="30" t="s"/>
-      <c r="L8" s="40" t="s">
+      <c r="I8" s="7" t="s"/>
+      <c r="J8" s="7" t="s"/>
+      <c r="K8" s="7" t="s"/>
+      <c r="L8" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="M8" s="30" t="s"/>
-      <c r="N8" s="30" t="s"/>
-      <c r="O8" s="30" t="s"/>
+      <c r="M8" s="7" t="s"/>
+      <c r="N8" s="7" t="s"/>
+      <c r="O8" s="7" t="s"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="47" t="s">
         <v>394</v>
       </c>
-      <c r="D9" s="49" t="n">
+      <c r="D9" s="29" t="n">
         <v>2012</v>
       </c>
-      <c r="E9" s="6" t="s"/>
-      <c r="F9" s="6" t="s"/>
-      <c r="G9" s="12" t="s"/>
-      <c r="H9" s="38" t="s">
+      <c r="E9" s="56" t="s"/>
+      <c r="F9" s="56" t="s"/>
+      <c r="G9" s="34" t="s"/>
+      <c r="H9" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="I9" s="36" t="s"/>
-      <c r="J9" s="36" t="s"/>
-      <c r="K9" s="36" t="s"/>
-      <c r="L9" s="38" t="s">
+      <c r="I9" s="54" t="s"/>
+      <c r="J9" s="54" t="s"/>
+      <c r="K9" s="54" t="s"/>
+      <c r="L9" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="M9" s="36" t="s"/>
-      <c r="N9" s="36" t="s"/>
-      <c r="O9" s="36" t="s"/>
+      <c r="M9" s="54" t="s"/>
+      <c r="N9" s="54" t="s"/>
+      <c r="O9" s="54" t="s"/>
     </row>
     <row r="10" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C10" s="27" t="s"/>
-      <c r="D10" s="23" t="s">
+      <c r="C10" s="17" t="s"/>
+      <c r="D10" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="23" t="s"/>
-      <c r="F10" s="23" t="s"/>
-      <c r="G10" s="37" t="s"/>
-      <c r="H10" s="10" t="s">
+      <c r="E10" s="42" t="s"/>
+      <c r="F10" s="42" t="s"/>
+      <c r="G10" s="43" t="s"/>
+      <c r="H10" s="38" t="s">
         <v>399</v>
       </c>
-      <c r="I10" s="10" t="s"/>
-      <c r="J10" s="10" t="s"/>
-      <c r="K10" s="10" t="s"/>
-      <c r="L10" s="10" t="s">
+      <c r="I10" s="38" t="s"/>
+      <c r="J10" s="38" t="s"/>
+      <c r="K10" s="38" t="s"/>
+      <c r="L10" s="38" t="s">
         <v>399</v>
       </c>
-      <c r="M10" s="10" t="s"/>
-      <c r="N10" s="10" t="s"/>
-      <c r="O10" s="10" t="s"/>
+      <c r="M10" s="38" t="s"/>
+      <c r="N10" s="38" t="s"/>
+      <c r="O10" s="38" t="s"/>
     </row>
     <row r="11" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C11" s="27" t="s"/>
-      <c r="D11" s="23" t="s"/>
-      <c r="E11" s="23" t="s"/>
-      <c r="F11" s="23" t="s"/>
-      <c r="G11" s="37" t="s"/>
-      <c r="H11" s="21" t="s">
+      <c r="C11" s="17" t="s"/>
+      <c r="D11" s="42" t="s"/>
+      <c r="E11" s="42" t="s"/>
+      <c r="F11" s="42" t="s"/>
+      <c r="G11" s="43" t="s"/>
+      <c r="H11" s="33" t="s">
         <v>477</v>
       </c>
-      <c r="I11" s="21" t="s"/>
-      <c r="J11" s="21" t="s"/>
-      <c r="K11" s="21" t="s"/>
-      <c r="L11" s="21" t="s">
+      <c r="I11" s="33" t="s"/>
+      <c r="J11" s="33" t="s"/>
+      <c r="K11" s="33" t="s"/>
+      <c r="L11" s="33" t="s">
         <v>477</v>
       </c>
-      <c r="M11" s="21" t="s"/>
-      <c r="N11" s="21" t="s"/>
-      <c r="O11" s="21" t="s"/>
+      <c r="M11" s="33" t="s"/>
+      <c r="N11" s="33" t="s"/>
+      <c r="O11" s="33" t="s"/>
     </row>
     <row r="12" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C12" s="52" t="s"/>
-      <c r="D12" s="48" t="s">
+      <c r="C12" s="53" t="s"/>
+      <c r="D12" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="E12" s="31" t="s"/>
-      <c r="F12" s="31" t="s"/>
-      <c r="G12" s="51" t="s"/>
-      <c r="H12" s="9" t="s">
+      <c r="E12" s="50" t="s"/>
+      <c r="F12" s="50" t="s"/>
+      <c r="G12" s="11" t="s"/>
+      <c r="H12" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I12" s="1" t="s"/>
-      <c r="J12" s="55" t="s"/>
-      <c r="K12" s="14" t="s"/>
-      <c r="L12" s="9" t="s">
+      <c r="I12" s="44" t="s"/>
+      <c r="J12" s="10" t="s"/>
+      <c r="K12" s="15" t="s"/>
+      <c r="L12" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="M12" s="1" t="s"/>
-      <c r="N12" s="55" t="s"/>
-      <c r="O12" s="14" t="s"/>
+      <c r="M12" s="44" t="s"/>
+      <c r="N12" s="10" t="s"/>
+      <c r="O12" s="15" t="s"/>
     </row>
     <row r="13" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="D13" s="24" t="s"/>
-      <c r="E13" s="32" t="s"/>
-      <c r="F13" s="32" t="s"/>
-      <c r="G13" s="50" t="s"/>
-      <c r="H13" s="7" t="s"/>
-      <c r="I13" s="7" t="s"/>
-      <c r="J13" s="4" t="s"/>
-      <c r="K13" s="4" t="s"/>
-      <c r="L13" s="7" t="s"/>
-      <c r="M13" s="7" t="s"/>
-      <c r="N13" s="4" t="s"/>
-      <c r="O13" s="4" t="s"/>
+      <c r="D13" s="14" t="s"/>
+      <c r="E13" s="12" t="s"/>
+      <c r="F13" s="12" t="s"/>
+      <c r="G13" s="48" t="s"/>
+      <c r="H13" s="19" t="s"/>
+      <c r="I13" s="19" t="s"/>
+      <c r="J13" s="21" t="s"/>
+      <c r="K13" s="21" t="s"/>
+      <c r="L13" s="19" t="s"/>
+      <c r="M13" s="19" t="s"/>
+      <c r="N13" s="21" t="s"/>
+      <c r="O13" s="21" t="s"/>
     </row>
     <row r="14" customHeight="1" ht="85.5" spans="1:15">
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="41" t="s">
         <v>470</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="31" t="s">
         <v>466</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="37" t="s">
         <v>467</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="H14" s="53" t="s">
+      <c r="H14" s="41" t="s">
         <v>470</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="31" t="s">
         <v>466</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="37" t="s">
         <v>467</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="L14" s="53" t="s">
+      <c r="L14" s="41" t="s">
         <v>470</v>
       </c>
-      <c r="M14" s="43" t="s">
+      <c r="M14" s="31" t="s">
         <v>466</v>
       </c>
-      <c r="N14" s="25" t="s">
+      <c r="N14" s="37" t="s">
         <v>467</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="28" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="15" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C15" s="3" t="s"/>
-      <c r="D15" s="22" t="s"/>
-      <c r="E15" s="22" t="s"/>
-      <c r="F15" s="17" t="s"/>
-      <c r="G15" s="35" t="s"/>
-      <c r="H15" s="22" t="s"/>
-      <c r="I15" s="22" t="s"/>
-      <c r="J15" s="17" t="s"/>
-      <c r="K15" s="35" t="s"/>
-      <c r="L15" s="22" t="s"/>
-      <c r="M15" s="22" t="s"/>
-      <c r="N15" s="17" t="s"/>
-      <c r="O15" s="35" t="s"/>
+      <c r="C15" s="13" t="s"/>
+      <c r="D15" s="9" t="s"/>
+      <c r="E15" s="9" t="s"/>
+      <c r="F15" s="24" t="s"/>
+      <c r="G15" s="27" t="s"/>
+      <c r="H15" s="9" t="s"/>
+      <c r="I15" s="9" t="s"/>
+      <c r="J15" s="24" t="s"/>
+      <c r="K15" s="27" t="s"/>
+      <c r="L15" s="9" t="s"/>
+      <c r="M15" s="9" t="s"/>
+      <c r="N15" s="24" t="s"/>
+      <c r="O15" s="27" t="s"/>
     </row>
     <row r="16" customHeight="1" ht="31.5" spans="1:15">
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="52" t="s">
         <v>468</v>
       </c>
-      <c r="D16" s="42" t="s"/>
-      <c r="E16" s="5" t="s"/>
-      <c r="F16" s="5" t="s"/>
-      <c r="G16" s="41" t="s"/>
-      <c r="H16" s="39" t="s"/>
-      <c r="I16" s="5" t="s"/>
-      <c r="J16" s="5" t="s"/>
-      <c r="K16" s="41" t="s"/>
-      <c r="L16" s="39" t="s"/>
-      <c r="M16" s="5" t="s"/>
-      <c r="N16" s="5" t="s"/>
-      <c r="O16" s="41" t="s"/>
+      <c r="D16" s="45" t="s"/>
+      <c r="E16" s="35" t="s"/>
+      <c r="F16" s="35" t="s"/>
+      <c r="G16" s="16" t="s"/>
+      <c r="H16" s="58" t="s"/>
+      <c r="I16" s="35" t="s"/>
+      <c r="J16" s="35" t="s"/>
+      <c r="K16" s="16" t="s"/>
+      <c r="L16" s="58" t="s"/>
+      <c r="M16" s="35" t="s"/>
+      <c r="N16" s="35" t="s"/>
+      <c r="O16" s="16" t="s"/>
     </row>
     <row r="17" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C17" s="3" t="s"/>
-      <c r="D17" s="22" t="s"/>
-      <c r="E17" s="22" t="s"/>
-      <c r="F17" s="17" t="s"/>
-      <c r="G17" s="35" t="s"/>
-      <c r="H17" s="22" t="s"/>
-      <c r="I17" s="22" t="s"/>
-      <c r="J17" s="17" t="s"/>
-      <c r="K17" s="35" t="s"/>
-      <c r="L17" s="22" t="s"/>
-      <c r="M17" s="22" t="s"/>
-      <c r="N17" s="17" t="s"/>
-      <c r="O17" s="35" t="s"/>
+      <c r="C17" s="13" t="s"/>
+      <c r="D17" s="9" t="s"/>
+      <c r="E17" s="9" t="s"/>
+      <c r="F17" s="24" t="s"/>
+      <c r="G17" s="27" t="s"/>
+      <c r="H17" s="9" t="s"/>
+      <c r="I17" s="9" t="s"/>
+      <c r="J17" s="24" t="s"/>
+      <c r="K17" s="27" t="s"/>
+      <c r="L17" s="9" t="s"/>
+      <c r="M17" s="9" t="s"/>
+      <c r="N17" s="24" t="s"/>
+      <c r="O17" s="27" t="s"/>
     </row>
     <row r="18" customHeight="1" ht="90.0" spans="1:15">
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="36" t="s">
         <v>445</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="46" t="s">
         <v>459</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="H18" s="54" t="s">
+      <c r="H18" s="46" t="s">
         <v>459</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="46" t="s">
+      <c r="K18" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="L18" s="54" t="s">
+      <c r="L18" s="46" t="s">
         <v>459</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="46" t="s">
+      <c r="O18" s="1" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="19" customHeight="1" ht="15.75" spans="1:15">
-      <c r="C19" s="3" t="s"/>
-      <c r="D19" s="22" t="s"/>
-      <c r="E19" s="22" t="s"/>
-      <c r="F19" s="17" t="s"/>
-      <c r="G19" s="35" t="s"/>
-      <c r="H19" s="22" t="s"/>
-      <c r="I19" s="22" t="s"/>
-      <c r="J19" s="17" t="s"/>
-      <c r="K19" s="35" t="s"/>
-      <c r="L19" s="22" t="s"/>
-      <c r="M19" s="22" t="s"/>
-      <c r="N19" s="17" t="s"/>
-      <c r="O19" s="35" t="s"/>
+      <c r="C19" s="13" t="s"/>
+      <c r="D19" s="9" t="s"/>
+      <c r="E19" s="9" t="s"/>
+      <c r="F19" s="24" t="s"/>
+      <c r="G19" s="27" t="s"/>
+      <c r="H19" s="9" t="s"/>
+      <c r="I19" s="9" t="s"/>
+      <c r="J19" s="24" t="s"/>
+      <c r="K19" s="27" t="s"/>
+      <c r="L19" s="9" t="s"/>
+      <c r="M19" s="9" t="s"/>
+      <c r="N19" s="24" t="s"/>
+      <c r="O19" s="27" t="s"/>
     </row>
     <row r="20" customHeight="1" ht="90.0" spans="1:15">
       <c r="A20" t="s">
@@ -3135,23 +3135,23 @@
       <c r="B20" t="s">
         <v>242</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="32" t="s">
         <v>443</v>
       </c>
-      <c r="D20" s="42" t="s"/>
-      <c r="E20" s="5" t="s"/>
-      <c r="F20" s="5" t="s"/>
-      <c r="G20" s="41" t="s"/>
-      <c r="H20" s="39" t="s"/>
-      <c r="I20" s="5" t="s"/>
-      <c r="J20" s="5" t="s"/>
-      <c r="K20" s="41" t="s"/>
-      <c r="L20" s="39" t="e">
+      <c r="D20" s="45" t="s"/>
+      <c r="E20" s="35" t="s"/>
+      <c r="F20" s="35" t="s"/>
+      <c r="G20" s="16" t="s"/>
+      <c r="H20" s="58" t="s"/>
+      <c r="I20" s="35" t="s"/>
+      <c r="J20" s="35" t="s"/>
+      <c r="K20" s="16" t="s"/>
+      <c r="L20" s="58" t="e">
         <v>#NAME?</v>
       </c>
-      <c r="M20" s="5" t="s"/>
-      <c r="N20" s="5" t="s"/>
-      <c r="O20" s="41" t="s"/>
+      <c r="M20" s="35" t="s"/>
+      <c r="N20" s="35" t="s"/>
+      <c r="O20" s="16" t="s"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -3190,45 +3190,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="39" customWidth="true" max="39" width="9.1640625"/>
-    <col min="38" customWidth="true" max="38" width="9.1640625"/>
-    <col min="35" customWidth="true" max="35" width="9.1640625"/>
-    <col min="34" customWidth="true" max="34" width="9.1640625"/>
-    <col min="37" customWidth="true" max="37" width="9.1640625"/>
-    <col min="36" customWidth="true" max="36" width="9.1640625"/>
-    <col min="31" customWidth="true" max="31" width="9.1640625"/>
-    <col min="30" customWidth="true" max="30" width="9.1640625"/>
-    <col min="33" customWidth="true" max="33" width="9.1640625"/>
-    <col min="32" customWidth="true" max="32" width="9.1640625"/>
-    <col min="27" customWidth="true" max="27" width="9.1640625"/>
-    <col min="29" customWidth="true" max="29" width="9.1640625"/>
-    <col min="28" customWidth="true" max="28" width="9.1640625"/>
-    <col min="21" customWidth="true" max="21" width="9.1640625"/>
-    <col min="20" customWidth="true" max="20" width="9.1640625"/>
-    <col min="23" customWidth="true" max="23" width="9.1640625"/>
-    <col min="22" customWidth="true" max="22" width="9.1640625"/>
-    <col min="17" customWidth="true" max="17" width="9.1640625"/>
-    <col min="16" customWidth="true" max="16" width="9.1640625"/>
-    <col min="19" customWidth="true" max="19" width="9.1640625"/>
-    <col min="18" customWidth="true" max="18" width="9.1640625"/>
-    <col min="25" customWidth="true" max="25" width="9.1640625"/>
-    <col min="24" customWidth="true" max="24" width="9.1640625"/>
-    <col min="26" customWidth="true" max="26" width="9.1640625"/>
-    <col min="5" customWidth="true" max="5" width="9.1640625"/>
-    <col min="4" customWidth="true" max="4" width="9.1640625"/>
-    <col min="7" customWidth="true" max="7" width="9.1640625"/>
-    <col min="6" customWidth="true" max="6" width="9.1640625"/>
-    <col min="1" customWidth="true" max="1" width="9.1640625"/>
-    <col min="3" customWidth="true" max="3" width="9.1640625"/>
-    <col min="2" customWidth="true" max="2" width="9.1640625"/>
-    <col min="13" customWidth="true" max="13" width="9.1640625"/>
-    <col min="12" customWidth="true" max="12" width="9.1640625"/>
-    <col min="15" customWidth="true" max="15" width="9.1640625"/>
-    <col min="14" customWidth="true" max="14" width="9.1640625"/>
-    <col min="9" customWidth="true" max="9" width="9.1640625"/>
-    <col min="8" customWidth="true" max="8" width="9.1640625"/>
-    <col min="11" customWidth="true" max="11" width="9.1640625"/>
-    <col min="10" customWidth="true" max="10" width="9.1640625"/>
+    <col min="5" width="9.1640625" max="5" customWidth="true"/>
+    <col min="4" width="9.1640625" max="4" customWidth="true"/>
+    <col min="7" width="9.1640625" max="7" customWidth="true"/>
+    <col min="6" width="9.1640625" max="6" customWidth="true"/>
+    <col min="1" width="9.1640625" max="1" customWidth="true"/>
+    <col min="29" width="9.1640625" max="29" customWidth="true"/>
+    <col min="3" width="9.1640625" max="3" customWidth="true"/>
+    <col min="2" width="9.1640625" max="2" customWidth="true"/>
+    <col min="13" width="9.1640625" max="13" customWidth="true"/>
+    <col min="12" width="9.1640625" max="12" customWidth="true"/>
+    <col min="15" width="9.1640625" max="15" customWidth="true"/>
+    <col min="14" width="9.1640625" max="14" customWidth="true"/>
+    <col min="9" width="9.1640625" max="9" customWidth="true"/>
+    <col min="8" width="9.1640625" max="8" customWidth="true"/>
+    <col min="11" width="9.1640625" max="11" customWidth="true"/>
+    <col min="10" width="9.1640625" max="10" customWidth="true"/>
+    <col min="21" width="9.1640625" max="21" customWidth="true"/>
+    <col min="20" width="9.1640625" max="20" customWidth="true"/>
+    <col min="23" width="9.1640625" max="23" customWidth="true"/>
+    <col min="22" width="9.1640625" max="22" customWidth="true"/>
+    <col min="17" width="9.1640625" max="17" customWidth="true"/>
+    <col min="16" width="9.1640625" max="16" customWidth="true"/>
+    <col min="19" width="9.1640625" max="19" customWidth="true"/>
+    <col min="18" width="9.1640625" max="18" customWidth="true"/>
+    <col min="39" width="9.1640625" max="39" customWidth="true"/>
+    <col min="38" width="9.1640625" max="38" customWidth="true"/>
+    <col min="25" width="9.1640625" max="25" customWidth="true"/>
+    <col min="24" width="9.1640625" max="24" customWidth="true"/>
+    <col min="37" width="9.1640625" max="37" customWidth="true"/>
+    <col min="26" width="9.1640625" max="26" customWidth="true"/>
+    <col min="31" width="9.1640625" max="31" customWidth="true"/>
+    <col min="30" width="9.1640625" max="30" customWidth="true"/>
+    <col min="35" width="9.1640625" max="35" customWidth="true"/>
+    <col min="33" width="9.1640625" max="33" customWidth="true"/>
+    <col min="34" width="9.1640625" max="34" customWidth="true"/>
+    <col min="32" width="9.1640625" max="32" customWidth="true"/>
+    <col min="27" width="9.1640625" max="27" customWidth="true"/>
+    <col min="28" width="9.1640625" max="28" customWidth="true"/>
+    <col min="36" width="9.1640625" max="36" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
@@ -10269,86 +10269,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="51" customWidth="true" max="51" width="9.1"/>
-    <col min="50" customWidth="true" max="50" width="9.1"/>
-    <col min="52" customWidth="true" max="52" width="9.1"/>
-    <col min="47" customWidth="true" max="47" width="9.1"/>
-    <col min="46" customWidth="true" max="46" width="9.1"/>
-    <col min="49" customWidth="true" max="49" width="9.1"/>
-    <col min="48" customWidth="true" max="48" width="9.1"/>
-    <col min="43" customWidth="true" max="43" width="9.1"/>
-    <col min="42" customWidth="true" max="42" width="9.1"/>
-    <col min="45" customWidth="true" max="45" width="9.1"/>
-    <col min="44" customWidth="true" max="44" width="9.1"/>
-    <col min="39" customWidth="true" max="39" width="9.1"/>
-    <col min="38" customWidth="true" max="38" width="9.1"/>
-    <col min="41" customWidth="true" max="41" width="9.1"/>
-    <col min="40" customWidth="true" max="40" width="9.1"/>
-    <col min="35" customWidth="true" max="35" width="9.1"/>
-    <col min="34" customWidth="true" max="34" width="9.1"/>
-    <col min="37" customWidth="true" max="37" width="9.1"/>
-    <col min="36" customWidth="true" max="36" width="9.1"/>
-    <col min="31" customWidth="true" max="31" width="9.1"/>
-    <col min="30" customWidth="true" max="30" width="9.1"/>
-    <col min="33" customWidth="true" max="33" width="9.1"/>
-    <col min="32" customWidth="true" max="32" width="9.1"/>
-    <col min="27" customWidth="true" max="27" width="9.1"/>
-    <col min="29" customWidth="true" max="29" width="9.1"/>
-    <col min="28" customWidth="true" max="28" width="9.1"/>
-    <col min="21" customWidth="true" max="21" width="9.1"/>
-    <col min="20" customWidth="true" max="20" width="9.1"/>
-    <col min="23" customWidth="true" max="23" width="9.1"/>
-    <col min="22" customWidth="true" max="22" width="9.1"/>
-    <col min="17" customWidth="true" max="17" width="9.1"/>
-    <col min="16" customWidth="true" max="16" width="9.1"/>
-    <col min="19" customWidth="true" max="19" width="9.1"/>
-    <col min="18" customWidth="true" max="18" width="9.1"/>
-    <col min="25" customWidth="true" max="25" width="9.1"/>
-    <col min="24" customWidth="true" max="24" width="9.1"/>
-    <col min="26" customWidth="true" max="26" width="9.1"/>
-    <col min="5" customWidth="true" max="5" width="9.1"/>
-    <col min="4" customWidth="true" max="4" width="9.1"/>
-    <col min="7" customWidth="true" max="7" width="9.1"/>
-    <col min="6" customWidth="true" max="6" width="9.1"/>
-    <col min="1" customWidth="true" max="1" width="9.1"/>
-    <col min="3" customWidth="true" max="3" width="9.1"/>
-    <col min="2" customWidth="true" max="2" width="9.1"/>
-    <col min="13" customWidth="true" max="13" width="9.1"/>
-    <col min="12" customWidth="true" max="12" width="9.1"/>
-    <col min="15" customWidth="true" max="15" width="9.1"/>
-    <col min="14" customWidth="true" max="14" width="9.1"/>
-    <col min="9" customWidth="true" max="9" width="9.1"/>
-    <col min="8" customWidth="true" max="8" width="9.1"/>
-    <col min="11" customWidth="true" max="11" width="9.1"/>
-    <col min="10" customWidth="true" max="10" width="9.1"/>
-    <col min="72" customWidth="true" max="72" width="9.1"/>
-    <col min="73" customWidth="true" max="73" width="9.1"/>
-    <col min="74" customWidth="true" max="74" width="9.1"/>
-    <col min="75" customWidth="true" max="75" width="9.1"/>
-    <col min="68" customWidth="true" max="68" width="9.1"/>
-    <col min="69" customWidth="true" max="69" width="9.1"/>
-    <col min="70" customWidth="true" max="70" width="9.1"/>
-    <col min="71" customWidth="true" max="71" width="9.1"/>
-    <col min="79" customWidth="true" max="79" width="9.1"/>
-    <col min="76" customWidth="true" max="76" width="9.1"/>
-    <col min="77" customWidth="true" max="77" width="9.1"/>
-    <col min="78" customWidth="true" max="78" width="9.1"/>
-    <col min="56" customWidth="true" max="56" width="9.1"/>
-    <col min="57" customWidth="true" max="57" width="9.1"/>
-    <col min="58" customWidth="true" max="58" width="9.1"/>
-    <col min="59" customWidth="true" max="59" width="9.1"/>
-    <col min="53" customWidth="true" max="53" width="9.1"/>
-    <col min="54" customWidth="true" max="54" width="9.1"/>
-    <col min="55" customWidth="true" max="55" width="9.1"/>
-    <col min="64" customWidth="true" max="64" width="9.1"/>
-    <col min="65" customWidth="true" max="65" width="9.1"/>
-    <col min="66" customWidth="true" max="66" width="9.1"/>
-    <col min="67" customWidth="true" max="67" width="9.1"/>
-    <col min="60" customWidth="true" max="60" width="9.1"/>
-    <col min="61" customWidth="true" max="61" width="9.1"/>
-    <col min="62" customWidth="true" max="62" width="9.1"/>
-    <col min="63" customWidth="true" max="63" width="9.1"/>
-    <col min="80" customWidth="true" max="80" width="9.1"/>
+    <col min="64" width="9.1" max="64" customWidth="true"/>
+    <col min="47" width="9.1" max="47" customWidth="true"/>
+    <col min="66" width="9.1" max="66" customWidth="true"/>
+    <col min="67" width="9.1" max="67" customWidth="true"/>
+    <col min="60" width="9.1" max="60" customWidth="true"/>
+    <col min="19" width="9.1" max="19" customWidth="true"/>
+    <col min="62" width="9.1" max="62" customWidth="true"/>
+    <col min="46" width="9.1" max="46" customWidth="true"/>
+    <col min="56" width="9.1" max="56" customWidth="true"/>
+    <col min="57" width="9.1" max="57" customWidth="true"/>
+    <col min="52" width="9.1" max="52" customWidth="true"/>
+    <col min="28" width="9.1" max="28" customWidth="true"/>
+    <col min="49" width="9.1" max="49" customWidth="true"/>
+    <col min="54" width="9.1" max="54" customWidth="true"/>
+    <col min="55" width="9.1" max="55" customWidth="true"/>
+    <col min="48" width="9.1" max="48" customWidth="true"/>
+    <col min="76" width="9.1" max="76" customWidth="true"/>
+    <col min="77" width="9.1" max="77" customWidth="true"/>
+    <col min="78" width="9.1" max="78" customWidth="true"/>
+    <col min="73" width="9.1" max="73" customWidth="true"/>
+    <col min="72" width="9.1" max="72" customWidth="true"/>
+    <col min="43" width="9.1" max="43" customWidth="true"/>
+    <col min="74" width="9.1" max="74" customWidth="true"/>
+    <col min="75" width="9.1" max="75" customWidth="true"/>
+    <col min="68" width="9.1" max="68" customWidth="true"/>
+    <col min="69" width="9.1" max="69" customWidth="true"/>
+    <col min="70" width="9.1" max="70" customWidth="true"/>
+    <col min="61" width="9.1" max="61" customWidth="true"/>
+    <col min="59" width="9.1" max="59" customWidth="true"/>
+    <col min="45" width="9.1" max="45" customWidth="true"/>
+    <col min="35" width="9.1" max="35" customWidth="true"/>
+    <col min="44" width="9.1" max="44" customWidth="true"/>
+    <col min="63" width="9.1" max="63" customWidth="true"/>
+    <col min="34" width="9.1" max="34" customWidth="true"/>
+    <col min="51" width="9.1" max="51" customWidth="true"/>
+    <col min="36" width="9.1" max="36" customWidth="true"/>
+    <col min="58" width="9.1" max="58" customWidth="true"/>
+    <col min="5" width="9.1" max="5" customWidth="true"/>
+    <col min="4" width="9.1" max="4" customWidth="true"/>
+    <col min="7" width="9.1" max="7" customWidth="true"/>
+    <col min="6" width="9.1" max="6" customWidth="true"/>
+    <col min="1" width="9.1" max="1" customWidth="true"/>
+    <col min="42" width="9.1" max="42" customWidth="true"/>
+    <col min="3" width="9.1" max="3" customWidth="true"/>
+    <col min="2" width="9.1" max="2" customWidth="true"/>
+    <col min="13" width="9.1" max="13" customWidth="true"/>
+    <col min="12" width="9.1" max="12" customWidth="true"/>
+    <col min="15" width="9.1" max="15" customWidth="true"/>
+    <col min="14" width="9.1" max="14" customWidth="true"/>
+    <col min="9" width="9.1" max="9" customWidth="true"/>
+    <col min="8" width="9.1" max="8" customWidth="true"/>
+    <col min="11" width="9.1" max="11" customWidth="true"/>
+    <col min="10" width="9.1" max="10" customWidth="true"/>
+    <col min="21" width="9.1" max="21" customWidth="true"/>
+    <col min="20" width="9.1" max="20" customWidth="true"/>
+    <col min="23" width="9.1" max="23" customWidth="true"/>
+    <col min="22" width="9.1" max="22" customWidth="true"/>
+    <col min="17" width="9.1" max="17" customWidth="true"/>
+    <col min="16" width="9.1" max="16" customWidth="true"/>
+    <col min="29" width="9.1" max="29" customWidth="true"/>
+    <col min="18" width="9.1" max="18" customWidth="true"/>
+    <col min="39" width="9.1" max="39" customWidth="true"/>
+    <col min="38" width="9.1" max="38" customWidth="true"/>
+    <col min="41" width="9.1" max="41" customWidth="true"/>
+    <col min="40" width="9.1" max="40" customWidth="true"/>
+    <col min="25" width="9.1" max="25" customWidth="true"/>
+    <col min="24" width="9.1" max="24" customWidth="true"/>
+    <col min="37" width="9.1" max="37" customWidth="true"/>
+    <col min="26" width="9.1" max="26" customWidth="true"/>
+    <col min="53" width="9.1" max="53" customWidth="true"/>
+    <col min="31" width="9.1" max="31" customWidth="true"/>
+    <col min="30" width="9.1" max="30" customWidth="true"/>
+    <col min="50" width="9.1" max="50" customWidth="true"/>
+    <col min="33" width="9.1" max="33" customWidth="true"/>
+    <col min="32" width="9.1" max="32" customWidth="true"/>
+    <col min="65" width="9.1" max="65" customWidth="true"/>
+    <col min="27" width="9.1" max="27" customWidth="true"/>
+    <col min="80" width="9.1" max="80" customWidth="true"/>
+    <col min="71" width="9.1" max="71" customWidth="true"/>
+    <col min="79" width="9.1" max="79" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:80">
@@ -45962,33 +45962,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="27" customWidth="true" max="27" width="9.1"/>
-    <col min="21" customWidth="true" max="21" width="9.1"/>
-    <col min="20" customWidth="true" max="20" width="9.1"/>
-    <col min="23" customWidth="true" max="23" width="9.1"/>
-    <col min="22" customWidth="true" max="22" width="9.1"/>
-    <col min="17" customWidth="true" max="17" width="9.1"/>
-    <col min="16" customWidth="true" max="16" width="9.1"/>
-    <col min="19" customWidth="true" max="19" width="9.1"/>
-    <col min="18" customWidth="true" max="18" width="9.1"/>
-    <col min="25" customWidth="true" max="25" width="9.1"/>
-    <col min="24" customWidth="true" max="24" width="9.1"/>
-    <col min="26" customWidth="true" max="26" width="9.1"/>
-    <col min="5" customWidth="true" max="5" width="9.1"/>
-    <col min="4" customWidth="true" max="4" width="9.1"/>
-    <col min="7" customWidth="true" max="7" width="9.1"/>
-    <col min="6" customWidth="true" max="6" width="9.1"/>
-    <col min="1" customWidth="true" max="1" width="9.1"/>
-    <col min="3" customWidth="true" max="3" width="9.1"/>
-    <col min="2" customWidth="true" max="2" width="9.1"/>
-    <col min="13" customWidth="true" max="13" width="9.1"/>
-    <col min="12" customWidth="true" max="12" width="9.1"/>
-    <col min="15" customWidth="true" max="15" width="9.1"/>
-    <col min="14" customWidth="true" max="14" width="9.1"/>
-    <col min="9" customWidth="true" max="9" width="9.1"/>
-    <col min="8" customWidth="true" max="8" width="9.1"/>
-    <col min="11" customWidth="true" max="11" width="9.1"/>
-    <col min="10" customWidth="true" max="10" width="9.1"/>
+    <col min="5" width="9.1" max="5" customWidth="true"/>
+    <col min="4" width="9.1" max="4" customWidth="true"/>
+    <col min="7" width="9.1" max="7" customWidth="true"/>
+    <col min="6" width="9.1" max="6" customWidth="true"/>
+    <col min="1" width="9.1" max="1" customWidth="true"/>
+    <col min="3" width="9.1" max="3" customWidth="true"/>
+    <col min="2" width="9.1" max="2" customWidth="true"/>
+    <col min="13" width="9.1" max="13" customWidth="true"/>
+    <col min="12" width="9.1" max="12" customWidth="true"/>
+    <col min="15" width="9.1" max="15" customWidth="true"/>
+    <col min="14" width="9.1" max="14" customWidth="true"/>
+    <col min="9" width="9.1" max="9" customWidth="true"/>
+    <col min="8" width="9.1" max="8" customWidth="true"/>
+    <col min="11" width="9.1" max="11" customWidth="true"/>
+    <col min="10" width="9.1" max="10" customWidth="true"/>
+    <col min="21" width="9.1" max="21" customWidth="true"/>
+    <col min="20" width="9.1" max="20" customWidth="true"/>
+    <col min="23" width="9.1" max="23" customWidth="true"/>
+    <col min="22" width="9.1" max="22" customWidth="true"/>
+    <col min="17" width="9.1" max="17" customWidth="true"/>
+    <col min="16" width="9.1" max="16" customWidth="true"/>
+    <col min="19" width="9.1" max="19" customWidth="true"/>
+    <col min="18" width="9.1" max="18" customWidth="true"/>
+    <col min="25" width="9.1" max="25" customWidth="true"/>
+    <col min="24" width="9.1" max="24" customWidth="true"/>
+    <col min="26" width="9.1" max="26" customWidth="true"/>
+    <col min="27" width="9.1" max="27" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -46107,6 +46107,9 @@
       <c r="O3" t="s">
         <v>448</v>
       </c>
+      <c r="P3" t="s">
+        <v>440</v>
+      </c>
       <c r="R3" t="s">
         <v>448</v>
       </c>
@@ -46151,6 +46154,9 @@
       <c r="O4" t="s">
         <v>440</v>
       </c>
+      <c r="P4" t="s">
+        <v>448</v>
+      </c>
       <c r="R4" t="s">
         <v>440</v>
       </c>
@@ -46171,12 +46177,6 @@
       <c r="A5" t="s">
         <v>246</v>
       </c>
-      <c r="D5" t="s">
-        <v>440</v>
-      </c>
-      <c r="G5" t="s">
-        <v>440</v>
-      </c>
       <c r="R5" t="s">
         <v>440</v>
       </c>
@@ -46185,25 +46185,7 @@
       <c r="A6" t="s">
         <v>247</v>
       </c>
-      <c r="B6" t="s">
-        <v>440</v>
-      </c>
-      <c r="D6" t="s">
-        <v>440</v>
-      </c>
-      <c r="F6" t="s">
-        <v>440</v>
-      </c>
-      <c r="G6" t="s">
-        <v>440</v>
-      </c>
-      <c r="K6" t="s">
-        <v>440</v>
-      </c>
       <c r="M6" t="s">
-        <v>440</v>
-      </c>
-      <c r="Q6" t="s">
         <v>440</v>
       </c>
       <c r="R6" t="s">
@@ -46222,9 +46204,6 @@
       <c r="F8" t="s">
         <v>448</v>
       </c>
-      <c r="L8" t="s">
-        <v>448</v>
-      </c>
       <c r="W8" t="s">
         <v>448</v>
       </c>
@@ -46236,9 +46215,6 @@
       <c r="A9" t="s">
         <v>250</v>
       </c>
-      <c r="K9" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="10" spans="1:27">
       <c r="A10" t="s">
@@ -46250,22 +46226,13 @@
       <c r="W10" t="s">
         <v>448</v>
       </c>
-      <c r="X10" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" t="s">
         <v>252</v>
       </c>
-      <c r="D11" t="s">
-        <v>448</v>
-      </c>
       <c r="L11" t="s">
         <v>448</v>
-      </c>
-      <c r="X11" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -46277,9 +46244,6 @@
       <c r="A13" t="s">
         <v>254</v>
       </c>
-      <c r="C13" t="s">
-        <v>448</v>
-      </c>
       <c r="L13" t="s">
         <v>448</v>
       </c>
@@ -46294,15 +46258,6 @@
       <c r="C14" t="s">
         <v>440</v>
       </c>
-      <c r="D14" t="s">
-        <v>440</v>
-      </c>
-      <c r="G14" t="s">
-        <v>440</v>
-      </c>
-      <c r="H14" t="s">
-        <v>440</v>
-      </c>
       <c r="K14" t="s">
         <v>440</v>
       </c>
@@ -46347,13 +46302,7 @@
       <c r="O15" t="s">
         <v>440</v>
       </c>
-      <c r="P15" t="s">
-        <v>440</v>
-      </c>
       <c r="R15" t="s">
-        <v>440</v>
-      </c>
-      <c r="W15" t="s">
         <v>440</v>
       </c>
       <c r="X15" t="s">
@@ -46373,18 +46322,9 @@
       <c r="C16" t="s">
         <v>440</v>
       </c>
-      <c r="E16" t="s">
-        <v>440</v>
-      </c>
       <c r="G16" t="s">
         <v>440</v>
       </c>
-      <c r="H16" t="s">
-        <v>440</v>
-      </c>
-      <c r="I16" t="s">
-        <v>440</v>
-      </c>
       <c r="K16" t="s">
         <v>440</v>
       </c>
@@ -46392,12 +46332,6 @@
         <v>440</v>
       </c>
       <c r="P16" t="s">
-        <v>440</v>
-      </c>
-      <c r="R16" t="s">
-        <v>440</v>
-      </c>
-      <c r="W16" t="s">
         <v>440</v>
       </c>
       <c r="X16" t="s">
@@ -46417,9 +46351,6 @@
       <c r="A17" t="s">
         <v>258</v>
       </c>
-      <c r="B17" t="s">
-        <v>448</v>
-      </c>
       <c r="C17" t="s">
         <v>448</v>
       </c>
@@ -46432,12 +46363,6 @@
       <c r="G17" t="s">
         <v>448</v>
       </c>
-      <c r="H17" t="s">
-        <v>448</v>
-      </c>
-      <c r="I17" t="s">
-        <v>448</v>
-      </c>
       <c r="J17" t="s">
         <v>448</v>
       </c>
@@ -46466,9 +46391,6 @@
         <v>448</v>
       </c>
       <c r="V17" t="s">
-        <v>448</v>
-      </c>
-      <c r="W17" t="s">
         <v>448</v>
       </c>
       <c r="X17" t="s">
@@ -46497,16 +46419,7 @@
       <c r="D18" t="s">
         <v>448</v>
       </c>
-      <c r="F18" t="s">
-        <v>448</v>
-      </c>
       <c r="G18" t="s">
-        <v>448</v>
-      </c>
-      <c r="H18" t="s">
-        <v>448</v>
-      </c>
-      <c r="I18" t="s">
         <v>448</v>
       </c>
       <c r="J18" t="s">
@@ -46565,9 +46478,6 @@
       <c r="A19" t="s">
         <v>260</v>
       </c>
-      <c r="H19" t="s">
-        <v>448</v>
-      </c>
       <c r="M19" t="s">
         <v>448</v>
       </c>
@@ -46582,9 +46492,6 @@
       <c r="A20" t="s">
         <v>261</v>
       </c>
-      <c r="Q20" t="s">
-        <v>440</v>
-      </c>
       <c r="W20" t="s">
         <v>440</v>
       </c>
@@ -46605,12 +46512,6 @@
       <c r="A21" t="s">
         <v>262</v>
       </c>
-      <c r="Q21" t="s">
-        <v>440</v>
-      </c>
-      <c r="W21" t="s">
-        <v>440</v>
-      </c>
       <c r="X21" t="s">
         <v>448</v>
       </c>
@@ -46631,9 +46532,6 @@
       <c r="E22" t="s">
         <v>448</v>
       </c>
-      <c r="W22" t="s">
-        <v>440</v>
-      </c>
       <c r="X22" t="s">
         <v>448</v>
       </c>
@@ -46654,24 +46552,12 @@
       <c r="Y23" t="s">
         <v>440</v>
       </c>
-      <c r="Z23" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="24" spans="1:27">
       <c r="A24" t="s">
         <v>265</v>
       </c>
-      <c r="W24" t="s">
-        <v>440</v>
-      </c>
       <c r="X24" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA24" t="s">
         <v>440</v>
       </c>
     </row>
@@ -46682,9 +46568,6 @@
       <c r="L25" t="s">
         <v>440</v>
       </c>
-      <c r="W25" t="s">
-        <v>440</v>
-      </c>
       <c r="Z25" t="s">
         <v>448</v>
       </c>
@@ -46696,9 +46579,6 @@
       <c r="C26" t="s">
         <v>448</v>
       </c>
-      <c r="D26" t="s">
-        <v>448</v>
-      </c>
       <c r="E26" t="s">
         <v>448</v>
       </c>
@@ -46719,17 +46599,8 @@
       <c r="A27" t="s">
         <v>268</v>
       </c>
-      <c r="E27" t="s">
-        <v>448</v>
-      </c>
       <c r="M27" t="s">
         <v>448</v>
-      </c>
-      <c r="O27" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -46739,16 +46610,10 @@
       <c r="C28" t="s">
         <v>448</v>
       </c>
-      <c r="D28" t="s">
-        <v>448</v>
-      </c>
       <c r="L28" t="s">
         <v>448</v>
       </c>
       <c r="M28" t="s">
-        <v>448</v>
-      </c>
-      <c r="O28" t="s">
         <v>448</v>
       </c>
       <c r="P28" t="s">
@@ -46777,15 +46642,6 @@
       <c r="A29" t="s">
         <v>270</v>
       </c>
-      <c r="B29" t="s">
-        <v>440</v>
-      </c>
-      <c r="L29" t="s">
-        <v>440</v>
-      </c>
-      <c r="M29" t="s">
-        <v>440</v>
-      </c>
       <c r="U29" t="s">
         <v>440</v>
       </c>
@@ -46797,18 +46653,9 @@
       <c r="A30" t="s">
         <v>271</v>
       </c>
-      <c r="B30" t="s">
-        <v>440</v>
-      </c>
-      <c r="D30" t="s">
-        <v>440</v>
-      </c>
       <c r="E30" t="s">
         <v>440</v>
       </c>
-      <c r="I30" t="s">
-        <v>440</v>
-      </c>
       <c r="L30" t="s">
         <v>440</v>
       </c>
@@ -46818,12 +46665,6 @@
       <c r="N30" t="s">
         <v>440</v>
       </c>
-      <c r="O30" t="s">
-        <v>440</v>
-      </c>
-      <c r="R30" t="s">
-        <v>440</v>
-      </c>
       <c r="S30" t="s">
         <v>440</v>
       </c>
@@ -46834,9 +46675,6 @@
         <v>440</v>
       </c>
       <c r="Z30" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA30" t="s">
         <v>440</v>
       </c>
     </row>
@@ -46844,9 +46682,6 @@
       <c r="A31" t="s">
         <v>272</v>
       </c>
-      <c r="AA31" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="32" spans="1:27">
       <c r="A32" t="s">
@@ -46855,9 +46690,6 @@
       <c r="E32" t="s">
         <v>440</v>
       </c>
-      <c r="V32" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="33" spans="1:27">
       <c r="A33" t="s">
@@ -46866,9 +46698,6 @@
       <c r="K33" t="s">
         <v>448</v>
       </c>
-      <c r="L33" t="s">
-        <v>448</v>
-      </c>
       <c r="Z33" t="s">
         <v>448</v>
       </c>
@@ -46889,12 +46718,6 @@
       <c r="T34" t="s">
         <v>440</v>
       </c>
-      <c r="U34" t="s">
-        <v>440</v>
-      </c>
-      <c r="V34" t="s">
-        <v>440</v>
-      </c>
       <c r="X34" t="s">
         <v>448</v>
       </c>
@@ -46918,15 +46741,6 @@
       <c r="G35" t="s">
         <v>440</v>
       </c>
-      <c r="H35" t="s">
-        <v>440</v>
-      </c>
-      <c r="I35" t="s">
-        <v>440</v>
-      </c>
-      <c r="J35" t="s">
-        <v>440</v>
-      </c>
       <c r="K35" t="s">
         <v>440</v>
       </c>
@@ -46992,19 +46806,10 @@
       <c r="D36" t="s">
         <v>440</v>
       </c>
-      <c r="E36" t="s">
-        <v>440</v>
-      </c>
       <c r="F36" t="s">
         <v>440</v>
       </c>
       <c r="G36" t="s">
-        <v>440</v>
-      </c>
-      <c r="H36" t="s">
-        <v>440</v>
-      </c>
-      <c r="I36" t="s">
         <v>440</v>
       </c>
       <c r="J36" t="s">
@@ -47066,9 +46871,6 @@
       <c r="A37" t="s">
         <v>278</v>
       </c>
-      <c r="B37" t="s">
-        <v>440</v>
-      </c>
       <c r="C37" t="s">
         <v>440</v>
       </c>
@@ -47078,9 +46880,6 @@
       <c r="F37" t="s">
         <v>440</v>
       </c>
-      <c r="K37" t="s">
-        <v>440</v>
-      </c>
       <c r="M37" t="s">
         <v>440</v>
       </c>
@@ -47103,9 +46902,6 @@
         <v>440</v>
       </c>
       <c r="T37" t="s">
-        <v>440</v>
-      </c>
-      <c r="U37" t="s">
         <v>440</v>
       </c>
       <c r="X37" t="s">
@@ -47125,9 +46921,6 @@
       <c r="A38" t="s">
         <v>279</v>
       </c>
-      <c r="W38" t="s">
-        <v>440</v>
-      </c>
       <c r="X38" t="s">
         <v>448</v>
       </c>
@@ -47153,18 +46946,12 @@
       <c r="K40" t="s">
         <v>440</v>
       </c>
-      <c r="L40" t="s">
-        <v>440</v>
-      </c>
       <c r="O40" t="s">
         <v>440</v>
       </c>
       <c r="P40" t="s">
         <v>440</v>
       </c>
-      <c r="Q40" t="s">
-        <v>440</v>
-      </c>
       <c r="S40" t="s">
         <v>440</v>
       </c>
@@ -47176,9 +46963,6 @@
       </c>
       <c r="X40" t="s">
         <v>448</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:27">
@@ -47209,17 +46993,11 @@
       <c r="U41" t="s">
         <v>448</v>
       </c>
-      <c r="V41" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="42" spans="1:27">
       <c r="A42" t="s">
         <v>283</v>
       </c>
-      <c r="K42" t="s">
-        <v>440</v>
-      </c>
       <c r="M42" t="s">
         <v>448</v>
       </c>
@@ -47237,21 +47015,12 @@
       <c r="D43" t="s">
         <v>448</v>
       </c>
-      <c r="E43" t="s">
-        <v>448</v>
-      </c>
-      <c r="G43" t="s">
-        <v>448</v>
-      </c>
       <c r="J43" t="s">
         <v>448</v>
       </c>
       <c r="M43" t="s">
         <v>448</v>
       </c>
-      <c r="O43" t="s">
-        <v>448</v>
-      </c>
       <c r="P43" t="s">
         <v>448</v>
       </c>
@@ -47265,9 +47034,6 @@
         <v>448</v>
       </c>
       <c r="V43" t="s">
-        <v>448</v>
-      </c>
-      <c r="X43" t="s">
         <v>448</v>
       </c>
     </row>
@@ -47278,9 +47044,6 @@
       <c r="E44" t="s">
         <v>448</v>
       </c>
-      <c r="K44" t="s">
-        <v>440</v>
-      </c>
       <c r="S44" t="s">
         <v>440</v>
       </c>
@@ -47306,29 +47069,14 @@
       <c r="V46" t="s">
         <v>448</v>
       </c>
-      <c r="Y46" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>288</v>
       </c>
-      <c r="B47" t="s">
-        <v>440</v>
-      </c>
       <c r="C47" t="s">
         <v>440</v>
       </c>
-      <c r="D47" t="s">
-        <v>440</v>
-      </c>
-      <c r="H47" t="s">
-        <v>440</v>
-      </c>
-      <c r="J47" t="s">
-        <v>440</v>
-      </c>
       <c r="K47" t="s">
         <v>440</v>
       </c>
@@ -47341,9 +47089,6 @@
       <c r="N47" t="s">
         <v>440</v>
       </c>
-      <c r="O47" t="s">
-        <v>440</v>
-      </c>
       <c r="P47" t="s">
         <v>440</v>
       </c>
@@ -47351,12 +47096,6 @@
         <v>440</v>
       </c>
       <c r="U47" t="s">
-        <v>440</v>
-      </c>
-      <c r="V47" t="s">
-        <v>440</v>
-      </c>
-      <c r="W47" t="s">
         <v>440</v>
       </c>
       <c r="X47" t="s">
@@ -47367,28 +47106,16 @@
       <c r="A48" t="s">
         <v>289</v>
       </c>
-      <c r="K48" t="s">
-        <v>440</v>
-      </c>
       <c r="M48" t="s">
         <v>440</v>
       </c>
       <c r="N48" t="s">
         <v>440</v>
       </c>
-      <c r="P48" t="s">
-        <v>440</v>
-      </c>
       <c r="U48" t="s">
         <v>440</v>
       </c>
-      <c r="W48" t="s">
-        <v>440</v>
-      </c>
       <c r="X48" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z48" t="s">
         <v>440</v>
       </c>
     </row>
@@ -47399,15 +47126,9 @@
       <c r="B49" t="s">
         <v>440</v>
       </c>
-      <c r="D49" t="s">
-        <v>440</v>
-      </c>
       <c r="E49" t="s">
         <v>440</v>
       </c>
-      <c r="F49" t="s">
-        <v>440</v>
-      </c>
       <c r="J49" t="s">
         <v>440</v>
       </c>
@@ -47420,12 +47141,6 @@
       <c r="N49" t="s">
         <v>440</v>
       </c>
-      <c r="O49" t="s">
-        <v>440</v>
-      </c>
-      <c r="P49" t="s">
-        <v>440</v>
-      </c>
       <c r="Q49" t="s">
         <v>440</v>
       </c>
@@ -47433,9 +47148,6 @@
         <v>440</v>
       </c>
       <c r="V49" t="s">
-        <v>440</v>
-      </c>
-      <c r="W49" t="s">
         <v>440</v>
       </c>
     </row>
@@ -47446,9 +47158,6 @@
       <c r="C50" t="s">
         <v>448</v>
       </c>
-      <c r="J50" t="s">
-        <v>448</v>
-      </c>
       <c r="L50" t="s">
         <v>448</v>
       </c>
@@ -47617,22 +47326,13 @@
       <c r="A56" t="s">
         <v>297</v>
       </c>
-      <c r="L56" t="s">
-        <v>440</v>
-      </c>
       <c r="T56" t="s">
         <v>440</v>
       </c>
-      <c r="W56" t="s">
-        <v>440</v>
-      </c>
       <c r="X56" t="s">
         <v>448</v>
       </c>
       <c r="Z56" t="s">
-        <v>448</v>
-      </c>
-      <c r="AA56" t="s">
         <v>448</v>
       </c>
     </row>
@@ -47640,25 +47340,13 @@
       <c r="A57" t="s">
         <v>298</v>
       </c>
-      <c r="F57" t="s">
-        <v>448</v>
-      </c>
       <c r="M57" t="s">
         <v>448</v>
       </c>
-      <c r="Q57" t="s">
-        <v>448</v>
-      </c>
       <c r="X57" t="s">
         <v>448</v>
       </c>
-      <c r="Y57" t="s">
-        <v>448</v>
-      </c>
       <c r="Z57" t="s">
-        <v>448</v>
-      </c>
-      <c r="AA57" t="s">
         <v>448</v>
       </c>
     </row>
@@ -47666,12 +47354,6 @@
       <c r="A58" t="s">
         <v>299</v>
       </c>
-      <c r="E58" t="s">
-        <v>440</v>
-      </c>
-      <c r="G58" t="s">
-        <v>440</v>
-      </c>
       <c r="J58" t="s">
         <v>440</v>
       </c>
@@ -47682,12 +47364,6 @@
         <v>440</v>
       </c>
       <c r="T58" t="s">
-        <v>440</v>
-      </c>
-      <c r="U58" t="s">
-        <v>440</v>
-      </c>
-      <c r="W58" t="s">
         <v>440</v>
       </c>
       <c r="X58" t="s">
@@ -47704,9 +47380,6 @@
       <c r="D59" t="s">
         <v>440</v>
       </c>
-      <c r="E59" t="s">
-        <v>440</v>
-      </c>
       <c r="F59" t="s">
         <v>440</v>
       </c>
@@ -47728,9 +47401,6 @@
       <c r="N59" t="s">
         <v>440</v>
       </c>
-      <c r="O59" t="s">
-        <v>440</v>
-      </c>
       <c r="Q59" t="s">
         <v>440</v>
       </c>
@@ -47741,9 +47411,6 @@
         <v>440</v>
       </c>
       <c r="X59" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y59" t="s">
         <v>440</v>
       </c>
     </row>
@@ -47751,15 +47418,9 @@
       <c r="A60" t="s">
         <v>301</v>
       </c>
-      <c r="C60" t="s">
-        <v>440</v>
-      </c>
       <c r="D60" t="s">
         <v>440</v>
       </c>
-      <c r="F60" t="s">
-        <v>440</v>
-      </c>
       <c r="G60" t="s">
         <v>440</v>
       </c>
@@ -47772,13 +47433,7 @@
       <c r="Q60" t="s">
         <v>440</v>
       </c>
-      <c r="R60" t="s">
-        <v>440</v>
-      </c>
       <c r="T60" t="s">
-        <v>440</v>
-      </c>
-      <c r="U60" t="s">
         <v>440</v>
       </c>
       <c r="X60" t="s">
@@ -47795,12 +47450,6 @@
       <c r="C61" t="s">
         <v>440</v>
       </c>
-      <c r="G61" t="s">
-        <v>440</v>
-      </c>
-      <c r="H61" t="s">
-        <v>440</v>
-      </c>
       <c r="I61" t="s">
         <v>440</v>
       </c>
@@ -47820,9 +47469,6 @@
         <v>440</v>
       </c>
       <c r="T61" t="s">
-        <v>440</v>
-      </c>
-      <c r="V61" t="s">
         <v>440</v>
       </c>
       <c r="X61" t="s">
@@ -47836,16 +47482,7 @@
       <c r="A62" t="s">
         <v>303</v>
       </c>
-      <c r="G62" t="s">
-        <v>448</v>
-      </c>
       <c r="Q62" t="s">
-        <v>440</v>
-      </c>
-      <c r="V62" t="s">
-        <v>440</v>
-      </c>
-      <c r="W62" t="s">
         <v>440</v>
       </c>
       <c r="X62" t="s">
@@ -47865,15 +47502,6 @@
       <c r="A63" t="s">
         <v>304</v>
       </c>
-      <c r="F63" t="s">
-        <v>440</v>
-      </c>
-      <c r="I63" t="s">
-        <v>440</v>
-      </c>
-      <c r="J63" t="s">
-        <v>440</v>
-      </c>
       <c r="M63" t="s">
         <v>440</v>
       </c>
@@ -47881,15 +47509,6 @@
         <v>440</v>
       </c>
       <c r="R63" t="s">
-        <v>440</v>
-      </c>
-      <c r="V63" t="s">
-        <v>440</v>
-      </c>
-      <c r="W63" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y63" t="s">
         <v>440</v>
       </c>
       <c r="Z63" t="s">
@@ -47912,9 +47531,6 @@
       <c r="Y64" t="s">
         <v>440</v>
       </c>
-      <c r="Z64" t="s">
-        <v>440</v>
-      </c>
       <c r="AA64" t="s">
         <v>440</v>
       </c>
@@ -47926,19 +47542,10 @@
       <c r="B65" t="s">
         <v>440</v>
       </c>
-      <c r="D65" t="s">
-        <v>440</v>
-      </c>
       <c r="F65" t="s">
         <v>440</v>
       </c>
       <c r="G65" t="s">
-        <v>440</v>
-      </c>
-      <c r="I65" t="s">
-        <v>440</v>
-      </c>
-      <c r="J65" t="s">
         <v>440</v>
       </c>
       <c r="Q65" t="s">
@@ -47958,22 +47565,10 @@
       <c r="A66" t="s">
         <v>307</v>
       </c>
-      <c r="B66" t="s">
-        <v>440</v>
-      </c>
-      <c r="D66" t="s">
-        <v>440</v>
-      </c>
       <c r="G66" t="s">
         <v>440</v>
       </c>
-      <c r="I66" t="s">
-        <v>440</v>
-      </c>
       <c r="Q66" t="s">
-        <v>440</v>
-      </c>
-      <c r="R66" t="s">
         <v>440</v>
       </c>
       <c r="T66" t="s">
@@ -47996,9 +47591,6 @@
       <c r="K67" t="s">
         <v>448</v>
       </c>
-      <c r="Q67" t="s">
-        <v>440</v>
-      </c>
       <c r="V67" t="s">
         <v>440</v>
       </c>
@@ -48007,12 +47599,6 @@
       <c r="A68" t="s">
         <v>309</v>
       </c>
-      <c r="N68" t="s">
-        <v>440</v>
-      </c>
-      <c r="W68" t="s">
-        <v>440</v>
-      </c>
       <c r="Z68" t="s">
         <v>440</v>
       </c>
@@ -48024,13 +47610,7 @@
       <c r="A69" t="s">
         <v>310</v>
       </c>
-      <c r="B69" t="s">
-        <v>440</v>
-      </c>
       <c r="N69" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z69" t="s">
         <v>440</v>
       </c>
     </row>
@@ -48038,12 +47618,6 @@
       <c r="A70" t="s">
         <v>311</v>
       </c>
-      <c r="B70" t="s">
-        <v>448</v>
-      </c>
-      <c r="W70" t="s">
-        <v>440</v>
-      </c>
       <c r="Z70" t="s">
         <v>440</v>
       </c>
@@ -48052,20 +47626,11 @@
       <c r="A71" t="s">
         <v>312</v>
       </c>
-      <c r="S71" t="s">
-        <v>448</v>
-      </c>
-      <c r="U71" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="72" spans="1:27">
       <c r="A72" t="s">
         <v>313</v>
       </c>
-      <c r="U72" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="73" spans="1:27">
       <c r="A73" t="s">
@@ -48100,9 +47665,6 @@
       <c r="R74" t="s">
         <v>440</v>
       </c>
-      <c r="W74" t="s">
-        <v>448</v>
-      </c>
       <c r="X74" t="s">
         <v>448</v>
       </c>
@@ -48114,23 +47676,14 @@
       <c r="B75" t="s">
         <v>440</v>
       </c>
-      <c r="D75" t="s">
-        <v>440</v>
-      </c>
       <c r="M75" t="s">
         <v>440</v>
       </c>
       <c r="N75" t="s">
         <v>440</v>
       </c>
-      <c r="P75" t="s">
-        <v>440</v>
-      </c>
       <c r="R75" t="s">
         <v>440</v>
-      </c>
-      <c r="W75" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="76" spans="1:27">
@@ -48140,9 +47693,6 @@
       <c r="B76" t="s">
         <v>440</v>
       </c>
-      <c r="D76" t="s">
-        <v>440</v>
-      </c>
       <c r="G76" t="s">
         <v>440</v>
       </c>
@@ -48163,21 +47713,9 @@
       <c r="C77" t="s">
         <v>440</v>
       </c>
-      <c r="D77" t="s">
-        <v>440</v>
-      </c>
-      <c r="E77" t="s">
-        <v>440</v>
-      </c>
       <c r="F77" t="s">
         <v>440</v>
       </c>
-      <c r="G77" t="s">
-        <v>440</v>
-      </c>
-      <c r="I77" t="s">
-        <v>440</v>
-      </c>
       <c r="J77" t="s">
         <v>440</v>
       </c>
@@ -48209,12 +47747,6 @@
         <v>440</v>
       </c>
       <c r="U77" t="s">
-        <v>440</v>
-      </c>
-      <c r="V77" t="s">
-        <v>440</v>
-      </c>
-      <c r="W77" t="s">
         <v>440</v>
       </c>
       <c r="X77" t="s">
@@ -48234,27 +47766,12 @@
       <c r="A78" t="s">
         <v>319</v>
       </c>
-      <c r="B78" t="s">
-        <v>440</v>
-      </c>
       <c r="C78" t="s">
         <v>440</v>
       </c>
-      <c r="D78" t="s">
-        <v>440</v>
-      </c>
       <c r="E78" t="s">
         <v>440</v>
       </c>
-      <c r="F78" t="s">
-        <v>440</v>
-      </c>
-      <c r="G78" t="s">
-        <v>440</v>
-      </c>
-      <c r="I78" t="s">
-        <v>440</v>
-      </c>
       <c r="J78" t="s">
         <v>440</v>
       </c>
@@ -48262,18 +47779,6 @@
         <v>440</v>
       </c>
       <c r="M78" t="s">
-        <v>440</v>
-      </c>
-      <c r="W78" t="s">
-        <v>440</v>
-      </c>
-      <c r="X78" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y78" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z78" t="s">
         <v>440</v>
       </c>
     </row>
@@ -48287,9 +47792,6 @@
       <c r="F79" t="s">
         <v>440</v>
       </c>
-      <c r="J79" t="s">
-        <v>440</v>
-      </c>
       <c r="K79" t="s">
         <v>440</v>
       </c>
@@ -48318,9 +47820,6 @@
         <v>440</v>
       </c>
       <c r="X79" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y79" t="s">
         <v>440</v>
       </c>
       <c r="AA79" t="s">
@@ -48334,12 +47833,6 @@
       <c r="B80" t="s">
         <v>448</v>
       </c>
-      <c r="C80" t="s">
-        <v>448</v>
-      </c>
-      <c r="I80" t="s">
-        <v>448</v>
-      </c>
       <c r="J80" t="s">
         <v>448</v>
       </c>
@@ -48368,9 +47861,6 @@
         <v>448</v>
       </c>
       <c r="T80" t="s">
-        <v>448</v>
-      </c>
-      <c r="V80" t="s">
         <v>448</v>
       </c>
       <c r="X80" t="s">
@@ -48416,12 +47906,6 @@
       <c r="B82" t="s">
         <v>448</v>
       </c>
-      <c r="H82" t="s">
-        <v>448</v>
-      </c>
-      <c r="I82" t="s">
-        <v>448</v>
-      </c>
       <c r="J82" t="s">
         <v>448</v>
       </c>
@@ -48466,16 +47950,10 @@
       <c r="P83" t="s">
         <v>448</v>
       </c>
-      <c r="R83" t="s">
-        <v>448</v>
-      </c>
       <c r="S83" t="s">
         <v>448</v>
       </c>
       <c r="T83" t="s">
-        <v>448</v>
-      </c>
-      <c r="V83" t="s">
         <v>448</v>
       </c>
       <c r="X83" t="s">
@@ -48542,9 +48020,6 @@
       <c r="V85" t="s">
         <v>448</v>
       </c>
-      <c r="W85" t="s">
-        <v>448</v>
-      </c>
       <c r="X85" t="s">
         <v>448</v>
       </c>
@@ -48710,9 +48185,6 @@
       <c r="O88" t="s">
         <v>448</v>
       </c>
-      <c r="Q88" t="s">
-        <v>448</v>
-      </c>
       <c r="S88" t="s">
         <v>448</v>
       </c>
@@ -48726,9 +48198,6 @@
         <v>448</v>
       </c>
       <c r="Y88" t="s">
-        <v>448</v>
-      </c>
-      <c r="Z88" t="s">
         <v>448</v>
       </c>
       <c r="AA88" t="s">
@@ -48739,26 +48208,14 @@
       <c r="A89" t="s">
         <v>330</v>
       </c>
-      <c r="J89" t="s">
-        <v>448</v>
-      </c>
-      <c r="O89" t="s">
-        <v>440</v>
-      </c>
       <c r="P89" t="s">
         <v>440</v>
       </c>
-      <c r="S89" t="s">
-        <v>440</v>
-      </c>
       <c r="W89" t="s">
         <v>440</v>
       </c>
       <c r="X89" t="s">
         <v>448</v>
-      </c>
-      <c r="Y89" t="s">
-        <v>440</v>
       </c>
       <c r="Z89" t="s">
         <v>440</v>
@@ -48782,22 +48239,10 @@
       <c r="A91" t="s">
         <v>332</v>
       </c>
-      <c r="J91" t="s">
-        <v>448</v>
-      </c>
       <c r="O91" t="s">
         <v>440</v>
       </c>
       <c r="P91" t="s">
-        <v>440</v>
-      </c>
-      <c r="S91" t="s">
-        <v>440</v>
-      </c>
-      <c r="W91" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y91" t="s">
         <v>440</v>
       </c>
       <c r="Z91" t="s">
@@ -48855,9 +48300,6 @@
       <c r="A93" t="s">
         <v>334</v>
       </c>
-      <c r="J93" t="s">
-        <v>448</v>
-      </c>
       <c r="K93" t="s">
         <v>440</v>
       </c>
@@ -48890,9 +48332,6 @@
       <c r="G94" t="s">
         <v>448</v>
       </c>
-      <c r="H94" t="s">
-        <v>448</v>
-      </c>
       <c r="I94" t="s">
         <v>448</v>
       </c>
@@ -48912,9 +48351,6 @@
         <v>448</v>
       </c>
       <c r="T94" t="s">
-        <v>448</v>
-      </c>
-      <c r="U94" t="s">
         <v>448</v>
       </c>
       <c r="V94" t="s">
@@ -48940,18 +48376,6 @@
       <c r="E95" t="s">
         <v>440</v>
       </c>
-      <c r="G95" t="s">
-        <v>440</v>
-      </c>
-      <c r="H95" t="s">
-        <v>440</v>
-      </c>
-      <c r="I95" t="s">
-        <v>440</v>
-      </c>
-      <c r="J95" t="s">
-        <v>440</v>
-      </c>
       <c r="K95" t="s">
         <v>440</v>
       </c>
@@ -48967,19 +48391,10 @@
       <c r="O95" t="s">
         <v>440</v>
       </c>
-      <c r="R95" t="s">
-        <v>440</v>
-      </c>
       <c r="T95" t="s">
         <v>440</v>
       </c>
-      <c r="V95" t="s">
-        <v>440</v>
-      </c>
       <c r="X95" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y95" t="s">
         <v>440</v>
       </c>
       <c r="Z95" t="s">
@@ -48996,12 +48411,6 @@
       <c r="B96" t="s">
         <v>440</v>
       </c>
-      <c r="E96" t="s">
-        <v>440</v>
-      </c>
-      <c r="L96" t="s">
-        <v>440</v>
-      </c>
       <c r="X96" t="s">
         <v>440</v>
       </c>
@@ -49022,12 +48431,6 @@
       <c r="E97" t="s">
         <v>440</v>
       </c>
-      <c r="H97" t="s">
-        <v>440</v>
-      </c>
-      <c r="J97" t="s">
-        <v>440</v>
-      </c>
       <c r="K97" t="s">
         <v>440</v>
       </c>
@@ -49047,9 +48450,6 @@
         <v>440</v>
       </c>
       <c r="X97" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y97" t="s">
         <v>440</v>
       </c>
       <c r="Z97" t="s">
@@ -49063,12 +48463,6 @@
       <c r="A98" t="s">
         <v>339</v>
       </c>
-      <c r="D98" t="s">
-        <v>448</v>
-      </c>
-      <c r="G98" t="s">
-        <v>448</v>
-      </c>
       <c r="L98" t="s">
         <v>448</v>
       </c>
@@ -49089,21 +48483,12 @@
       <c r="A99" t="s">
         <v>340</v>
       </c>
+      <c r="C99" t="s">
+        <v>448</v>
+      </c>
       <c r="D99" t="s">
         <v>448</v>
       </c>
-      <c r="F99" t="s">
-        <v>448</v>
-      </c>
-      <c r="G99" t="s">
-        <v>448</v>
-      </c>
-      <c r="H99" t="s">
-        <v>448</v>
-      </c>
-      <c r="I99" t="s">
-        <v>448</v>
-      </c>
       <c r="L99" t="s">
         <v>448</v>
       </c>
@@ -49114,9 +48499,6 @@
         <v>448</v>
       </c>
       <c r="T99" t="s">
-        <v>448</v>
-      </c>
-      <c r="V99" t="s">
         <v>448</v>
       </c>
       <c r="X99" t="s">
@@ -49135,9 +48517,6 @@
       <c r="C101" t="s">
         <v>448</v>
       </c>
-      <c r="G101" t="s">
-        <v>448</v>
-      </c>
       <c r="M101" t="s">
         <v>448</v>
       </c>
@@ -49162,13 +48541,7 @@
       <c r="U101" t="s">
         <v>448</v>
       </c>
-      <c r="V101" t="s">
-        <v>448</v>
-      </c>
       <c r="W101" t="s">
-        <v>448</v>
-      </c>
-      <c r="Y101" t="s">
         <v>448</v>
       </c>
       <c r="AA101" t="s">
@@ -49212,9 +48585,6 @@
       <c r="W102" t="s">
         <v>448</v>
       </c>
-      <c r="Y102" t="s">
-        <v>448</v>
-      </c>
       <c r="Z102" t="s">
         <v>448</v>
       </c>
@@ -49226,16 +48596,10 @@
       <c r="A103" t="s">
         <v>344</v>
       </c>
-      <c r="I103" t="s">
-        <v>440</v>
-      </c>
       <c r="O103" t="s">
         <v>448</v>
       </c>
       <c r="P103" t="s">
-        <v>448</v>
-      </c>
-      <c r="Q103" t="s">
         <v>448</v>
       </c>
       <c r="R103" t="s">
@@ -49251,16 +48615,10 @@
       <c r="A105" t="s">
         <v>346</v>
       </c>
-      <c r="C105" t="s">
-        <v>440</v>
-      </c>
       <c r="O105" t="s">
         <v>440</v>
       </c>
       <c r="T105" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA105" t="s">
         <v>440</v>
       </c>
     </row>
@@ -49271,9 +48629,6 @@
       <c r="K106" t="s">
         <v>448</v>
       </c>
-      <c r="Y106" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="107" spans="1:27">
       <c r="A107" t="s">
@@ -49282,9 +48637,6 @@
       <c r="K107" t="s">
         <v>448</v>
       </c>
-      <c r="L107" t="s">
-        <v>440</v>
-      </c>
       <c r="O107" t="s">
         <v>448</v>
       </c>
@@ -49295,9 +48647,6 @@
         <v>448</v>
       </c>
       <c r="V107" t="s">
-        <v>440</v>
-      </c>
-      <c r="W107" t="s">
         <v>440</v>
       </c>
       <c r="X107" t="s">
@@ -49314,9 +48663,6 @@
       <c r="A108" t="s">
         <v>349</v>
       </c>
-      <c r="K108" t="s">
-        <v>448</v>
-      </c>
       <c r="L108" t="s">
         <v>440</v>
       </c>
@@ -49324,9 +48670,6 @@
         <v>448</v>
       </c>
       <c r="T108" t="s">
-        <v>440</v>
-      </c>
-      <c r="V108" t="s">
         <v>440</v>
       </c>
       <c r="X108" t="s">
@@ -49343,9 +48686,6 @@
       <c r="A109" t="s">
         <v>350</v>
       </c>
-      <c r="E109" t="s">
-        <v>448</v>
-      </c>
       <c r="F109" t="s">
         <v>448</v>
       </c>
@@ -49353,9 +48693,6 @@
         <v>448</v>
       </c>
       <c r="N109" t="s">
-        <v>448</v>
-      </c>
-      <c r="P109" t="s">
         <v>448</v>
       </c>
       <c r="U109" t="s">
@@ -49375,17 +48712,11 @@
       <c r="S110" t="s">
         <v>448</v>
       </c>
-      <c r="W110" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="111" spans="1:27">
       <c r="A111" t="s">
         <v>352</v>
       </c>
-      <c r="H111" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="112" spans="1:27">
       <c r="A112" t="s">
@@ -49421,9 +48752,6 @@
       <c r="A115" t="s">
         <v>356</v>
       </c>
-      <c r="O115" t="s">
-        <v>440</v>
-      </c>
       <c r="X115" t="s">
         <v>448</v>
       </c>
@@ -49435,24 +48763,12 @@
       <c r="C116" t="s">
         <v>440</v>
       </c>
-      <c r="D116" t="s">
-        <v>440</v>
-      </c>
       <c r="G116" t="s">
         <v>440</v>
       </c>
-      <c r="H116" t="s">
-        <v>440</v>
-      </c>
-      <c r="I116" t="s">
-        <v>440</v>
-      </c>
       <c r="K116" t="s">
         <v>440</v>
       </c>
-      <c r="L116" t="s">
-        <v>440</v>
-      </c>
       <c r="M116" t="s">
         <v>440</v>
       </c>
@@ -49465,16 +48781,10 @@
       <c r="R116" t="s">
         <v>440</v>
       </c>
-      <c r="S116" t="s">
-        <v>440</v>
-      </c>
       <c r="T116" t="s">
         <v>440</v>
       </c>
       <c r="X116" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y116" t="s">
         <v>440</v>
       </c>
       <c r="Z116" t="s">
@@ -49488,12 +48798,6 @@
       <c r="A117" t="s">
         <v>358</v>
       </c>
-      <c r="C117" t="s">
-        <v>440</v>
-      </c>
-      <c r="G117" t="s">
-        <v>440</v>
-      </c>
       <c r="K117" t="s">
         <v>440</v>
       </c>
@@ -49503,9 +48807,6 @@
       <c r="N117" t="s">
         <v>440</v>
       </c>
-      <c r="O117" t="s">
-        <v>440</v>
-      </c>
       <c r="Q117" t="s">
         <v>440</v>
       </c>
@@ -49516,9 +48817,6 @@
         <v>440</v>
       </c>
       <c r="T117" t="s">
-        <v>440</v>
-      </c>
-      <c r="W117" t="s">
         <v>440</v>
       </c>
       <c r="X117" t="s">
@@ -49532,9 +48830,6 @@
       <c r="A118" t="s">
         <v>359</v>
       </c>
-      <c r="I118" t="s">
-        <v>440</v>
-      </c>
       <c r="M118" t="s">
         <v>440</v>
       </c>
@@ -49552,9 +48847,6 @@
       <c r="O119" t="s">
         <v>440</v>
       </c>
-      <c r="P119" t="s">
-        <v>440</v>
-      </c>
       <c r="T119" t="s">
         <v>448</v>
       </c>
@@ -49566,9 +48858,6 @@
       <c r="G120" t="s">
         <v>448</v>
       </c>
-      <c r="M120" t="s">
-        <v>448</v>
-      </c>
       <c r="T120" t="s">
         <v>448</v>
       </c>
@@ -49577,15 +48866,6 @@
       <c r="A121" t="s">
         <v>362</v>
       </c>
-      <c r="C121" t="s">
-        <v>448</v>
-      </c>
-      <c r="I121" t="s">
-        <v>448</v>
-      </c>
-      <c r="P121" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="122" spans="1:27">
       <c r="A122" t="s">
@@ -49597,13 +48877,7 @@
       <c r="U122" t="s">
         <v>440</v>
       </c>
-      <c r="W122" t="s">
-        <v>440</v>
-      </c>
       <c r="X122" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y122" t="s">
         <v>440</v>
       </c>
     </row>
@@ -49619,19 +48893,10 @@
       <c r="A124" t="s">
         <v>365</v>
       </c>
-      <c r="H124" t="s">
-        <v>440</v>
-      </c>
       <c r="U124" t="s">
         <v>440</v>
       </c>
-      <c r="W124" t="s">
-        <v>440</v>
-      </c>
       <c r="X124" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y124" t="s">
         <v>440</v>
       </c>
     </row>
@@ -49642,12 +48907,6 @@
       <c r="G125" t="s">
         <v>440</v>
       </c>
-      <c r="J125" t="s">
-        <v>448</v>
-      </c>
-      <c r="P125" t="s">
-        <v>440</v>
-      </c>
       <c r="X125" t="s">
         <v>448</v>
       </c>
@@ -49664,23 +48923,11 @@
       <c r="G127" t="s">
         <v>440</v>
       </c>
-      <c r="P127" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="128" spans="1:27">
       <c r="A128" t="s">
         <v>369</v>
       </c>
-      <c r="B128" t="s">
-        <v>440</v>
-      </c>
-      <c r="D128" t="s">
-        <v>440</v>
-      </c>
-      <c r="E128" t="s">
-        <v>440</v>
-      </c>
       <c r="M128" t="s">
         <v>440</v>
       </c>
@@ -49707,15 +48954,9 @@
       <c r="C129" t="s">
         <v>440</v>
       </c>
-      <c r="D129" t="s">
-        <v>440</v>
-      </c>
       <c r="E129" t="s">
         <v>440</v>
       </c>
-      <c r="K129" t="s">
-        <v>440</v>
-      </c>
       <c r="M129" t="s">
         <v>440</v>
       </c>
@@ -49735,9 +48976,6 @@
         <v>440</v>
       </c>
       <c r="T129" t="s">
-        <v>440</v>
-      </c>
-      <c r="U129" t="s">
         <v>440</v>
       </c>
     </row>
@@ -49751,30 +48989,15 @@
       <c r="R130" t="s">
         <v>440</v>
       </c>
-      <c r="S130" t="s">
-        <v>440</v>
-      </c>
-      <c r="T130" t="s">
-        <v>448</v>
-      </c>
-      <c r="U130" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="131" spans="1:27">
       <c r="A131" t="s">
         <v>372</v>
       </c>
-      <c r="K131" t="s">
-        <v>440</v>
-      </c>
       <c r="L131" t="s">
         <v>440</v>
       </c>
       <c r="N131" t="s">
-        <v>440</v>
-      </c>
-      <c r="O131" t="s">
         <v>440</v>
       </c>
     </row>
@@ -49785,32 +49008,11 @@
       <c r="E132" t="s">
         <v>448</v>
       </c>
-      <c r="K132" t="s">
-        <v>440</v>
-      </c>
-      <c r="L132" t="s">
-        <v>440</v>
-      </c>
-      <c r="O132" t="s">
-        <v>440</v>
-      </c>
-      <c r="R132" t="s">
-        <v>440</v>
-      </c>
-      <c r="V132" t="s">
-        <v>448</v>
-      </c>
-      <c r="X132" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="133" spans="1:27">
       <c r="A133" t="s">
         <v>374</v>
       </c>
-      <c r="L133" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="134" spans="1:27">
       <c r="A134" t="s">
@@ -49825,9 +49027,6 @@
       <c r="G134" t="s">
         <v>448</v>
       </c>
-      <c r="H134" t="s">
-        <v>448</v>
-      </c>
       <c r="I134" t="s">
         <v>448</v>
       </c>
@@ -49896,9 +49095,6 @@
       <c r="R135" t="s">
         <v>448</v>
       </c>
-      <c r="V135" t="s">
-        <v>448</v>
-      </c>
       <c r="W135" t="s">
         <v>448</v>
       </c>
@@ -49925,9 +49121,6 @@
       <c r="G136" t="s">
         <v>448</v>
       </c>
-      <c r="H136" t="s">
-        <v>448</v>
-      </c>
       <c r="I136" t="s">
         <v>448</v>
       </c>
@@ -49956,9 +49149,6 @@
         <v>448</v>
       </c>
       <c r="V136" t="s">
-        <v>448</v>
-      </c>
-      <c r="W136" t="s">
         <v>448</v>
       </c>
       <c r="Y136" t="s">
@@ -49984,9 +49174,6 @@
       <c r="D137" t="s">
         <v>440</v>
       </c>
-      <c r="H137" t="s">
-        <v>440</v>
-      </c>
       <c r="K137" t="s">
         <v>440</v>
       </c>
@@ -50006,9 +49193,6 @@
         <v>440</v>
       </c>
       <c r="Q137" t="s">
-        <v>440</v>
-      </c>
-      <c r="R137" t="s">
         <v>440</v>
       </c>
       <c r="S137" t="s">
@@ -50034,21 +49218,12 @@
       <c r="A138" t="s">
         <v>379</v>
       </c>
-      <c r="B138" t="s">
-        <v>440</v>
-      </c>
       <c r="C138" t="s">
         <v>440</v>
       </c>
-      <c r="D138" t="s">
-        <v>440</v>
-      </c>
       <c r="K138" t="s">
         <v>440</v>
       </c>
-      <c r="L138" t="s">
-        <v>440</v>
-      </c>
       <c r="M138" t="s">
         <v>440</v>
       </c>
@@ -50064,9 +49239,6 @@
       <c r="Q138" t="s">
         <v>440</v>
       </c>
-      <c r="R138" t="s">
-        <v>440</v>
-      </c>
       <c r="S138" t="s">
         <v>440</v>
       </c>
@@ -50077,12 +49249,6 @@
         <v>440</v>
       </c>
       <c r="Y138" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z138" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA138" t="s">
         <v>440</v>
       </c>
     </row>
@@ -50090,15 +49256,9 @@
       <c r="A139" t="s">
         <v>380</v>
       </c>
-      <c r="B139" t="s">
-        <v>440</v>
-      </c>
       <c r="C139" t="s">
         <v>440</v>
       </c>
-      <c r="D139" t="s">
-        <v>440</v>
-      </c>
       <c r="E139" t="s">
         <v>448</v>
       </c>
@@ -50129,13 +49289,7 @@
       <c r="X139" t="s">
         <v>440</v>
       </c>
-      <c r="Y139" t="s">
-        <v>440</v>
-      </c>
       <c r="Z139" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA139" t="s">
         <v>440</v>
       </c>
     </row>
@@ -50155,19 +49309,10 @@
       <c r="P140" t="s">
         <v>440</v>
       </c>
-      <c r="Q140" t="s">
-        <v>440</v>
-      </c>
-      <c r="R140" t="s">
-        <v>440</v>
-      </c>
       <c r="S140" t="s">
         <v>440</v>
       </c>
       <c r="W140" t="s">
-        <v>440</v>
-      </c>
-      <c r="X140" t="s">
         <v>440</v>
       </c>
       <c r="Y140" t="s">
@@ -50190,15 +49335,6 @@
       <c r="K141" t="s">
         <v>440</v>
       </c>
-      <c r="O141" t="s">
-        <v>440</v>
-      </c>
-      <c r="W141" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y141" t="s">
-        <v>440</v>
-      </c>
       <c r="Z141" t="s">
         <v>440</v>
       </c>
@@ -50207,15 +49343,9 @@
       <c r="A142" t="s">
         <v>383</v>
       </c>
-      <c r="E142" t="s">
-        <v>440</v>
-      </c>
       <c r="K142" t="s">
         <v>440</v>
       </c>
-      <c r="L142" t="s">
-        <v>440</v>
-      </c>
       <c r="M142" t="s">
         <v>440</v>
       </c>
@@ -50234,16 +49364,7 @@
       <c r="U142" t="s">
         <v>440</v>
       </c>
-      <c r="W142" t="s">
-        <v>440</v>
-      </c>
       <c r="Y142" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z142" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA142" t="s">
         <v>440</v>
       </c>
     </row>
@@ -50259,13 +49380,7 @@
       <c r="A144" t="s">
         <v>385</v>
       </c>
-      <c r="E144" t="s">
-        <v>448</v>
-      </c>
       <c r="U144" t="s">
-        <v>448</v>
-      </c>
-      <c r="V144" t="s">
         <v>448</v>
       </c>
       <c r="X144" t="s">
@@ -50282,12 +49397,6 @@
       <c r="C145" t="s">
         <v>440</v>
       </c>
-      <c r="F145" t="s">
-        <v>440</v>
-      </c>
-      <c r="I145" t="s">
-        <v>440</v>
-      </c>
       <c r="K145" t="s">
         <v>440</v>
       </c>
@@ -50303,16 +49412,7 @@
       <c r="S145" t="s">
         <v>440</v>
       </c>
-      <c r="U145" t="s">
-        <v>440</v>
-      </c>
       <c r="W145" t="s">
-        <v>440</v>
-      </c>
-      <c r="Y145" t="s">
-        <v>440</v>
-      </c>
-      <c r="Z145" t="s">
         <v>440</v>
       </c>
     </row>
@@ -50320,12 +49420,6 @@
       <c r="A146" t="s">
         <v>387</v>
       </c>
-      <c r="O146" t="s">
-        <v>440</v>
-      </c>
-      <c r="AA146" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="147" spans="1:27">
       <c r="A147" t="s">
@@ -50334,16 +49428,10 @@
       <c r="O147" t="s">
         <v>440</v>
       </c>
-      <c r="P147" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="148" spans="1:27">
       <c r="A148" t="s">
         <v>389</v>
-      </c>
-      <c r="B148" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="149" spans="1:27">

</xml_diff>